<commit_message>
first round of character finding finished, some progress on adding the new keyboard
</commit_message>
<xml_diff>
--- a/Resources/TranslationKeys.xlsx
+++ b/Resources/TranslationKeys.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="396">
   <si>
     <t>Arabic Name</t>
   </si>
@@ -781,13 +781,439 @@
   </si>
   <si>
     <t>Blue = unfound, possibly unnecessary.</t>
+  </si>
+  <si>
+    <t>&amp;#xa2</t>
+  </si>
+  <si>
+    <t>Cent Sign</t>
+  </si>
+  <si>
+    <t>Arabic Start Of Rub El Hizb</t>
+  </si>
+  <si>
+    <t>&amp;#x6de</t>
+  </si>
+  <si>
+    <t>DIVISION SIGN</t>
+  </si>
+  <si>
+    <t>0x00F7</t>
+  </si>
+  <si>
+    <t>&amp;#x660</t>
+  </si>
+  <si>
+    <t>Arabic-Indic Digit Zero</t>
+  </si>
+  <si>
+    <t>&amp;#x661</t>
+  </si>
+  <si>
+    <t>&amp;#x662</t>
+  </si>
+  <si>
+    <t>&amp;#x663</t>
+  </si>
+  <si>
+    <t>&amp;#x664</t>
+  </si>
+  <si>
+    <t>&amp;#x665</t>
+  </si>
+  <si>
+    <t>&amp;#x666</t>
+  </si>
+  <si>
+    <t>&amp;#x667</t>
+  </si>
+  <si>
+    <t>&amp;#x668</t>
+  </si>
+  <si>
+    <t>&amp;#x669</t>
+  </si>
+  <si>
+    <t>Arabic-Indic Digit One</t>
+  </si>
+  <si>
+    <t>Arabic-Indic Digit Two</t>
+  </si>
+  <si>
+    <t>Arabic-Indic Digit Three</t>
+  </si>
+  <si>
+    <t>Arabic-Indic Digit Four</t>
+  </si>
+  <si>
+    <t>Arabic-Indic Digit Five</t>
+  </si>
+  <si>
+    <t>Arabic-Indic Digit Six</t>
+  </si>
+  <si>
+    <t>Arabic-Indic Digit Seven</t>
+  </si>
+  <si>
+    <t>Arabic-Indic Digit Eight</t>
+  </si>
+  <si>
+    <t>Arabic-Indic Digit Nine</t>
+  </si>
+  <si>
+    <t>commercial at</t>
+  </si>
+  <si>
+    <t>Number Sign</t>
+  </si>
+  <si>
+    <t>Dollar Sign</t>
+  </si>
+  <si>
+    <t>Percent sign</t>
+  </si>
+  <si>
+    <t>Conrol sign</t>
+  </si>
+  <si>
+    <t>ampersand</t>
+  </si>
+  <si>
+    <t>Asterisk</t>
+  </si>
+  <si>
+    <t>ARABIC FIVE POINTED STAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">002A </t>
+  </si>
+  <si>
+    <t>Dotted Line</t>
+  </si>
+  <si>
+    <t>"low minus"</t>
+  </si>
+  <si>
+    <t>"hyphen minus"</t>
+  </si>
+  <si>
+    <t>Plus sign</t>
+  </si>
+  <si>
+    <t>Equals sign</t>
+  </si>
+  <si>
+    <t>back slash</t>
+  </si>
+  <si>
+    <t>Arabic Number Sign</t>
+  </si>
+  <si>
+    <t>&amp;#x600</t>
+  </si>
+  <si>
+    <t>&amp;#x66f</t>
+  </si>
+  <si>
+    <t>Arabic Letter Dotless Qaf</t>
+  </si>
+  <si>
+    <t>Arabic Small High Jeem</t>
+  </si>
+  <si>
+    <t>&amp;#x6da</t>
+  </si>
+  <si>
+    <t>Arabic Small High Three Dots</t>
+  </si>
+  <si>
+    <t>&amp;#x6db</t>
+  </si>
+  <si>
+    <t>Arabic Small Waw</t>
+  </si>
+  <si>
+    <t>&amp;#x6e5</t>
+  </si>
+  <si>
+    <t>High Dots</t>
+  </si>
+  <si>
+    <t>REGISTERED SIGN</t>
+  </si>
+  <si>
+    <t>&amp;#00ae</t>
+  </si>
+  <si>
+    <t>Arabic Small High Noon</t>
+  </si>
+  <si>
+    <t>&amp;#x6e8</t>
+  </si>
+  <si>
+    <t>TRADE MARK SIGN</t>
+  </si>
+  <si>
+    <t>&amp;#2122</t>
+  </si>
+  <si>
+    <t>&amp;#x60f</t>
+  </si>
+  <si>
+    <t>Arabic Sign Misra</t>
+  </si>
+  <si>
+    <t>&amp;#x655</t>
+  </si>
+  <si>
+    <t>Arabic Hamza Below</t>
+  </si>
+  <si>
+    <t>YEN SIGN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;#00A5 </t>
+  </si>
+  <si>
+    <t>Arabic Ligature Qala Used As Koranic Stop Sign Isolated Form</t>
+  </si>
+  <si>
+    <t>&amp;#xfdf1</t>
+  </si>
+  <si>
+    <t>High Salla</t>
+  </si>
+  <si>
+    <t>High Yeh Baree</t>
+  </si>
+  <si>
+    <t>Arabic Letter Teh Marbuta</t>
+  </si>
+  <si>
+    <t>&amp;#x629</t>
+  </si>
+  <si>
+    <t>Arabic Letter Heh</t>
+  </si>
+  <si>
+    <t>&amp;#x647</t>
+  </si>
+  <si>
+    <t>POUND SIGN</t>
+  </si>
+  <si>
+    <t>&amp;#00A3</t>
+  </si>
+  <si>
+    <t>Arabic Percent Sign</t>
+  </si>
+  <si>
+    <t>&amp;#x66a</t>
+  </si>
+  <si>
+    <t>left curly bracket</t>
+  </si>
+  <si>
+    <t>right curly bracket</t>
+  </si>
+  <si>
+    <t>left ornate curly bracket</t>
+  </si>
+  <si>
+    <t>right ornate curly bracket</t>
+  </si>
+  <si>
+    <t>Arabic Ligature Allah Isolated Form</t>
+  </si>
+  <si>
+    <t>&amp;#xfdf2</t>
+  </si>
+  <si>
+    <t>Arabic Letter Alef Wasla</t>
+  </si>
+  <si>
+    <t>&amp;#x671</t>
+  </si>
+  <si>
+    <t>Arabic Ligature Salam Isolated Form</t>
+  </si>
+  <si>
+    <t>&amp;#xfdf5</t>
+  </si>
+  <si>
+    <t>Safa Sign</t>
+  </si>
+  <si>
+    <t>DEGREE SIGN</t>
+  </si>
+  <si>
+    <t>&amp;#00B0</t>
+  </si>
+  <si>
+    <t>Arabic Small High Seen</t>
+  </si>
+  <si>
+    <t>&amp;#x6dc</t>
+  </si>
+  <si>
+    <t>Arabic Small Low Seen</t>
+  </si>
+  <si>
+    <t>&amp;#x6e3</t>
+  </si>
+  <si>
+    <t>Arabic Letter Dotless Feh</t>
+  </si>
+  <si>
+    <t>&amp;#x6a1</t>
+  </si>
+  <si>
+    <t>VULGAR FRACTION ONE HALF</t>
+  </si>
+  <si>
+    <t>&amp;#00BD</t>
+  </si>
+  <si>
+    <t>VULGAR FRACTION ONE QUARTER</t>
+  </si>
+  <si>
+    <t>&amp;#00BC</t>
+  </si>
+  <si>
+    <t>&amp;#00BE</t>
+  </si>
+  <si>
+    <t>VULGAR FRACTION THREE QUARTERS</t>
+  </si>
+  <si>
+    <t>&amp;#x643</t>
+  </si>
+  <si>
+    <t>Arabic Letter Kaf</t>
+  </si>
+  <si>
+    <t>Dochashmi Hey</t>
+  </si>
+  <si>
+    <t>Arabic Ligature Jallajalalouhou</t>
+  </si>
+  <si>
+    <t>&amp;#xfdfb</t>
+  </si>
+  <si>
+    <t>Arabic Letter Swash Kaf</t>
+  </si>
+  <si>
+    <t>&amp;#x6aa</t>
+  </si>
+  <si>
+    <t>english semicolon</t>
+  </si>
+  <si>
+    <t>quote</t>
+  </si>
+  <si>
+    <t>apostrophe</t>
+  </si>
+  <si>
+    <t>Arabic Letter Veh</t>
+  </si>
+  <si>
+    <t>&amp;#x6a4</t>
+  </si>
+  <si>
+    <t>Arabic Small Low Meem</t>
+  </si>
+  <si>
+    <t>&amp;#x6ed</t>
+  </si>
+  <si>
+    <t>Arabic Small High Meem Isolated Form</t>
+  </si>
+  <si>
+    <t>&amp;#x6e2</t>
+  </si>
+  <si>
+    <t>Arabic Small High Meem Initial Form</t>
+  </si>
+  <si>
+    <t>&amp;#x6d8</t>
+  </si>
+  <si>
+    <t>&amp;#x6e9</t>
+  </si>
+  <si>
+    <t>Arabic Place Of Sajdah</t>
+  </si>
+  <si>
+    <t>COPYRIGHT SIGN</t>
+  </si>
+  <si>
+    <t>&amp;#00A9</t>
+  </si>
+  <si>
+    <t>Riyal sign</t>
+  </si>
+  <si>
+    <t>&amp;#x615</t>
+  </si>
+  <si>
+    <t>Arabic Small High Tah</t>
+  </si>
+  <si>
+    <t>&amp;#x66e</t>
+  </si>
+  <si>
+    <t>Arabic Letter Dotless Beh</t>
+  </si>
+  <si>
+    <t>Arabic Ligature Bismillah Ar-Rahman Ar-Raheem</t>
+  </si>
+  <si>
+    <t>&amp;#xfdfd</t>
+  </si>
+  <si>
+    <t>Arabic End Of Ayah</t>
+  </si>
+  <si>
+    <t>&amp;#x6dd</t>
+  </si>
+  <si>
+    <t>&amp;#x602</t>
+  </si>
+  <si>
+    <t>Arabic Footnote Marker</t>
+  </si>
+  <si>
+    <t>MULTIPLICATION X</t>
+  </si>
+  <si>
+    <t>&amp;#2715</t>
+  </si>
+  <si>
+    <t>Arabic Ligature Mohammad Isolated Form</t>
+  </si>
+  <si>
+    <t>&amp;#xfdf4</t>
+  </si>
+  <si>
+    <t>front slash</t>
+  </si>
+  <si>
+    <t>less than</t>
+  </si>
+  <si>
+    <t>greater than</t>
+  </si>
+  <si>
+    <t>question</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -812,6 +1238,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="MyriadPro"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -862,7 +1306,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -906,8 +1350,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -936,8 +1404,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -959,6 +1434,18 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -980,6 +1467,18 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1311,15 +1810,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:KE201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="C190" sqref="C190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="36.83203125" customWidth="1"/>
+    <col min="3" max="3" width="52.6640625" customWidth="1"/>
     <col min="4" max="5" width="10.83203125" style="10"/>
     <col min="6" max="6" width="12" style="10" customWidth="1"/>
     <col min="7" max="291" width="10.83203125" style="10"/>
@@ -9574,491 +10073,1021 @@
       <c r="A101" s="8" t="s">
         <v>2</v>
       </c>
+      <c r="B101" t="s">
+        <v>254</v>
+      </c>
+      <c r="C101" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="8" t="s">
         <v>3</v>
       </c>
+      <c r="B102" t="s">
+        <v>257</v>
+      </c>
+      <c r="C102" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="8" t="s">
         <v>4</v>
       </c>
+      <c r="B103" t="s">
+        <v>259</v>
+      </c>
+      <c r="C103" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" s="8">
         <v>1</v>
       </c>
+      <c r="B104" t="s">
+        <v>262</v>
+      </c>
+      <c r="C104" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="8" t="s">
         <v>5</v>
       </c>
+      <c r="B105" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="8">
         <v>2</v>
       </c>
+      <c r="B106" t="s">
+        <v>263</v>
+      </c>
+      <c r="C106" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="8" t="s">
         <v>6</v>
       </c>
+      <c r="B107" t="s">
+        <v>6</v>
+      </c>
+      <c r="C107" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="8">
         <v>3</v>
       </c>
+      <c r="B108" t="s">
+        <v>264</v>
+      </c>
+      <c r="C108" s="14" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="B109" t="s">
+        <v>7</v>
+      </c>
+      <c r="C109" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="8">
         <v>4</v>
       </c>
+      <c r="B110" t="s">
+        <v>265</v>
+      </c>
+      <c r="C110" s="14" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="B111" t="s">
+        <v>8</v>
+      </c>
+      <c r="C111" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="113" spans="1:1">
+      <c r="B112" t="s">
+        <v>266</v>
+      </c>
+      <c r="C112" s="14" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
       <c r="A113" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="114" spans="1:1">
+      <c r="B113" t="s">
+        <v>9</v>
+      </c>
+      <c r="C113" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
       <c r="A114" s="8">
         <v>6</v>
       </c>
-    </row>
-    <row r="115" spans="1:1">
+      <c r="B114" t="s">
+        <v>267</v>
+      </c>
+      <c r="C114" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
       <c r="A115" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="116" spans="1:1">
+      <c r="B115" t="s">
+        <v>10</v>
+      </c>
+      <c r="C115" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
       <c r="A116" s="8">
         <v>7</v>
       </c>
-    </row>
-    <row r="117" spans="1:1">
+      <c r="B116" t="s">
+        <v>268</v>
+      </c>
+      <c r="C116" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
       <c r="A117" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="118" spans="1:1">
+      <c r="B117" t="s">
+        <v>11</v>
+      </c>
+      <c r="C117" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
       <c r="A118" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="119" spans="1:1">
+      <c r="B118" t="s">
+        <v>269</v>
+      </c>
+      <c r="C118" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
       <c r="A119" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="120" spans="1:1">
+      <c r="B119" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="C119" s="15" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
       <c r="A120" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="121" spans="1:1">
-      <c r="A121" s="8" t="s">
+      <c r="B120" t="s">
+        <v>270</v>
+      </c>
+      <c r="C120" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="122" spans="1:1">
+      <c r="B121" s="17"/>
+      <c r="C121" s="17" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
       <c r="A122" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:1">
+      <c r="B122" t="s">
+        <v>260</v>
+      </c>
+      <c r="C122" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
       <c r="A123" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="124" spans="1:1">
+      <c r="B123" t="s">
+        <v>14</v>
+      </c>
+      <c r="C123" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
       <c r="A124" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="125" spans="1:1">
+      <c r="B124" t="s">
+        <v>15</v>
+      </c>
+      <c r="C124" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
       <c r="A125" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="126" spans="1:1">
+      <c r="B125" t="s">
+        <v>16</v>
+      </c>
+      <c r="C125" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
       <c r="A126" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="127" spans="1:1">
+      <c r="B126" t="s">
+        <v>17</v>
+      </c>
+      <c r="C126" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
       <c r="A127" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="128" spans="1:1">
+      <c r="B127" t="s">
+        <v>19</v>
+      </c>
+      <c r="C127" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
       <c r="A128" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="129" spans="1:1">
+      <c r="B128" t="s">
+        <v>296</v>
+      </c>
+      <c r="C128" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
       <c r="A129" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="130" spans="1:1">
+      <c r="B129" t="s">
+        <v>297</v>
+      </c>
+      <c r="C129" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
       <c r="A130" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="131" spans="1:1">
+      <c r="B130" t="s">
+        <v>300</v>
+      </c>
+      <c r="C130" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
       <c r="A131" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="132" spans="1:1">
+      <c r="B131" t="s">
+        <v>302</v>
+      </c>
+      <c r="C131" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
       <c r="A132" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="133" spans="1:1">
-      <c r="A133" s="8" t="s">
+      <c r="B132" t="s">
+        <v>304</v>
+      </c>
+      <c r="C132" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" s="10" customFormat="1">
+      <c r="A133" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="134" spans="1:1">
+      <c r="B133" s="5"/>
+      <c r="C133" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
       <c r="A134" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="135" spans="1:1">
+      <c r="B134" t="s">
+        <v>312</v>
+      </c>
+      <c r="C134" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
       <c r="A135" s="8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="136" spans="1:1">
+      <c r="B135" t="s">
+        <v>307</v>
+      </c>
+      <c r="C135" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
       <c r="A136" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="137" spans="1:1">
+      <c r="B136" t="s">
+        <v>309</v>
+      </c>
+      <c r="C136" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
       <c r="A137" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="138" spans="1:1">
+      <c r="B137" t="s">
+        <v>311</v>
+      </c>
+      <c r="C137" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
       <c r="A138" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="139" spans="1:1">
+      <c r="B138" t="s">
+        <v>314</v>
+      </c>
+      <c r="C138" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
       <c r="A139" s="8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="140" spans="1:1">
+      <c r="B139" t="s">
+        <v>317</v>
+      </c>
+      <c r="C139" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
       <c r="A140" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="141" spans="1:1">
+      <c r="B140" t="s">
+        <v>168</v>
+      </c>
+      <c r="C140" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
       <c r="A141" s="8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="142" spans="1:1">
+      <c r="B141" t="s">
+        <v>319</v>
+      </c>
+      <c r="C141" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
       <c r="A142" s="8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="143" spans="1:1">
-      <c r="A143" s="8" t="s">
+      <c r="B142" t="s">
+        <v>97</v>
+      </c>
+      <c r="C142" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="144" spans="1:1">
-      <c r="A144" s="8" t="s">
+      <c r="B143" s="5"/>
+      <c r="C143" s="5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="145" spans="1:1">
+      <c r="B144" s="5"/>
+      <c r="C144" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
       <c r="A145" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="146" spans="1:1">
+      <c r="B145" t="s">
+        <v>323</v>
+      </c>
+      <c r="C145" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
       <c r="A146" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="147" spans="1:1">
+      <c r="B146" t="s">
+        <v>325</v>
+      </c>
+      <c r="C146" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
       <c r="A147" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="148" spans="1:1">
+      <c r="B147" t="s">
+        <v>327</v>
+      </c>
+      <c r="C147" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
       <c r="A148" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="149" spans="1:1">
+      <c r="B148" t="s">
+        <v>329</v>
+      </c>
+      <c r="C148" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
       <c r="A149" s="8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="150" spans="1:1">
-      <c r="A150" s="8" t="s">
+      <c r="B149" t="s">
+        <v>40</v>
+      </c>
+      <c r="C149" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="151" spans="1:1">
+      <c r="B150" s="5"/>
+      <c r="C150" s="5" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
       <c r="A151" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="152" spans="1:1">
-      <c r="A152" s="8" t="s">
+      <c r="B151" t="s">
+        <v>42</v>
+      </c>
+      <c r="C151" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="153" spans="1:1">
+      <c r="B152" s="5"/>
+      <c r="C152" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
       <c r="A153" s="8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="154" spans="1:1">
+      <c r="B153" t="s">
+        <v>335</v>
+      </c>
+      <c r="C153" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
       <c r="A154" s="8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="155" spans="1:1">
+      <c r="B154" t="s">
+        <v>337</v>
+      </c>
+      <c r="C154" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
       <c r="A155" s="8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="156" spans="1:1">
-      <c r="A156" s="8" t="s">
+      <c r="B155" t="s">
+        <v>339</v>
+      </c>
+      <c r="C155" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" s="10" customFormat="1">
+      <c r="A156" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="157" spans="1:1">
+      <c r="B156" s="5"/>
+      <c r="C156" s="5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
       <c r="A157" s="8" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="158" spans="1:1">
+      <c r="B157" t="s">
+        <v>342</v>
+      </c>
+      <c r="C157" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
       <c r="A158" s="8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="159" spans="1:1">
+      <c r="B158" t="s">
+        <v>344</v>
+      </c>
+      <c r="C158" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
       <c r="A159" s="8" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="160" spans="1:1">
+      <c r="B159" t="s">
+        <v>348</v>
+      </c>
+      <c r="C159" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
       <c r="A160" s="8" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="161" spans="1:1">
+      <c r="B160" t="s">
+        <v>346</v>
+      </c>
+      <c r="C160" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
       <c r="A161" s="8" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="162" spans="1:1">
+      <c r="B161" t="s">
+        <v>352</v>
+      </c>
+      <c r="C161" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
       <c r="A162" s="8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="163" spans="1:1">
+      <c r="B162" t="s">
+        <v>355</v>
+      </c>
+      <c r="C162" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
       <c r="A163" s="8" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="164" spans="1:1">
-      <c r="A164" s="8" t="s">
+      <c r="B163" t="s">
+        <v>350</v>
+      </c>
+      <c r="C163" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="165" spans="1:1">
+      <c r="B164" s="5"/>
+      <c r="C164" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
       <c r="A165" s="8" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="166" spans="1:1">
+      <c r="B165" t="s">
+        <v>353</v>
+      </c>
+      <c r="C165" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
       <c r="A166" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="167" spans="1:1">
+      <c r="B166" t="s">
+        <v>359</v>
+      </c>
+      <c r="C166" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
       <c r="A167" s="8" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="168" spans="1:1">
+      <c r="B167" t="s">
+        <v>319</v>
+      </c>
+      <c r="C167" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
       <c r="A168" s="8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="169" spans="1:1">
-      <c r="A169" s="8" t="s">
+      <c r="B168" t="s">
+        <v>361</v>
+      </c>
+      <c r="C168" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="170" spans="1:1">
-      <c r="A170" s="8" t="s">
+      <c r="B169" s="5"/>
+      <c r="C169" s="5"/>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="171" spans="1:1">
+      <c r="B170" s="5"/>
+      <c r="C170" s="5"/>
+    </row>
+    <row r="171" spans="1:3">
       <c r="A171" s="8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="172" spans="1:1">
+      <c r="B171" t="s">
+        <v>186</v>
+      </c>
+      <c r="C171" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
       <c r="A172" s="8" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="173" spans="1:1">
+      <c r="B172" t="s">
+        <v>63</v>
+      </c>
+      <c r="C172" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
       <c r="A173" s="8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="174" spans="1:1">
+      <c r="B173" t="s">
+        <v>64</v>
+      </c>
+      <c r="C173" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
       <c r="A174" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="175" spans="1:1">
+      <c r="B174" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C174" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
       <c r="A175" s="8" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="176" spans="1:1">
+      <c r="B175" t="s">
+        <v>366</v>
+      </c>
+      <c r="C175" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
       <c r="A176" s="8" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="177" spans="1:1">
+      <c r="B176" t="s">
+        <v>370</v>
+      </c>
+      <c r="C176" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
       <c r="A177" s="8" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="178" spans="1:1">
+      <c r="B177" t="s">
+        <v>373</v>
+      </c>
+      <c r="C177" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
       <c r="A178" s="8" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="179" spans="1:1">
+      <c r="B178" t="s">
+        <v>368</v>
+      </c>
+      <c r="C178" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
       <c r="A179" s="8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="180" spans="1:1">
+      <c r="B179" t="s">
+        <v>376</v>
+      </c>
+      <c r="C179" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
       <c r="A180" s="8" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="181" spans="1:1">
-      <c r="A181" s="8" t="s">
+      <c r="B180" t="s">
+        <v>372</v>
+      </c>
+      <c r="C180" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="182" spans="1:1">
+      <c r="B181" s="5"/>
+      <c r="C181" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
       <c r="A182" s="8" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="183" spans="1:1">
+      <c r="B182" t="s">
+        <v>378</v>
+      </c>
+      <c r="C182" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
       <c r="A183" s="8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="184" spans="1:1">
+      <c r="B183" t="s">
+        <v>380</v>
+      </c>
+      <c r="C183" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
       <c r="A184" s="8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="185" spans="1:1">
+      <c r="B184" t="s">
+        <v>383</v>
+      </c>
+      <c r="C184" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
       <c r="A185" s="8" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="186" spans="1:1">
+      <c r="B185" t="s">
+        <v>385</v>
+      </c>
+      <c r="C185" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
       <c r="A186" s="8" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="187" spans="1:1">
+      <c r="B186" t="s">
+        <v>386</v>
+      </c>
+      <c r="C186" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
       <c r="A187" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="188" spans="1:1">
-      <c r="A188" s="8" t="s">
+      <c r="B187" t="s">
+        <v>389</v>
+      </c>
+      <c r="C187" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" s="10" customFormat="1">
+      <c r="A188" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="189" spans="1:1">
+      <c r="B188" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
       <c r="A189" s="8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="190" spans="1:1">
-      <c r="A190" s="8" t="s">
+      <c r="B189" t="s">
+        <v>80</v>
+      </c>
+      <c r="C189" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="191" spans="1:1">
+      <c r="B190" s="3"/>
+      <c r="C190" s="3"/>
+    </row>
+    <row r="191" spans="1:3">
       <c r="A191" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="192" spans="1:1">
-      <c r="A192" s="8" t="s">
+      <c r="B191" t="s">
+        <v>84</v>
+      </c>
+      <c r="C191" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="193" spans="1:1">
+      <c r="B192" s="3"/>
+      <c r="C192" s="3"/>
+    </row>
+    <row r="193" spans="1:3">
       <c r="A193" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="194" spans="1:1">
+      <c r="B193" t="s">
+        <v>84</v>
+      </c>
+      <c r="C193" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
       <c r="A194" s="8" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="195" spans="1:1">
+      <c r="B194" t="s">
+        <v>85</v>
+      </c>
+      <c r="C194" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
       <c r="A195" s="8"/>
     </row>
-    <row r="196" spans="1:1">
+    <row r="196" spans="1:3">
       <c r="A196" s="8"/>
     </row>
-    <row r="197" spans="1:1">
+    <row r="197" spans="1:3">
       <c r="A197" s="8"/>
     </row>
-    <row r="198" spans="1:1">
+    <row r="198" spans="1:3">
       <c r="A198" s="8"/>
     </row>
-    <row r="199" spans="1:1">
+    <row r="199" spans="1:3">
       <c r="A199" s="8"/>
     </row>
-    <row r="200" spans="1:1">
+    <row r="200" spans="1:3">
       <c r="A200" s="8"/>
     </row>
-    <row r="201" spans="1:1">
+    <row r="201" spans="1:3">
       <c r="A201" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Have a new keyboard currently under "ab" with some letters changed on a testing basis. Also, found more unicode values.
</commit_message>
<xml_diff>
--- a/Resources/TranslationKeys.xlsx
+++ b/Resources/TranslationKeys.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="415">
   <si>
     <t>Arabic Name</t>
   </si>
@@ -324,12 +324,6 @@
     <t>&amp;#x66c</t>
   </si>
   <si>
-    <t>Arabic Letter Yeh</t>
-  </si>
-  <si>
-    <t>&amp;#x64a</t>
-  </si>
-  <si>
     <t>&amp;#x6af</t>
   </si>
   <si>
@@ -645,9 +639,6 @@
     <t>Rehmat Sign</t>
   </si>
   <si>
-    <t>Laam</t>
-  </si>
-  <si>
     <t>colon</t>
   </si>
   <si>
@@ -936,9 +927,6 @@
     <t>&amp;#x6e5</t>
   </si>
   <si>
-    <t>High Dots</t>
-  </si>
-  <si>
     <t>REGISTERED SIGN</t>
   </si>
   <si>
@@ -981,9 +969,6 @@
     <t>&amp;#xfdf1</t>
   </si>
   <si>
-    <t>High Salla</t>
-  </si>
-  <si>
     <t>High Yeh Baree</t>
   </si>
   <si>
@@ -1041,9 +1026,6 @@
     <t>&amp;#xfdf5</t>
   </si>
   <si>
-    <t>Safa Sign</t>
-  </si>
-  <si>
     <t>DEGREE SIGN</t>
   </si>
   <si>
@@ -1092,9 +1074,6 @@
     <t>Arabic Letter Kaf</t>
   </si>
   <si>
-    <t>Dochashmi Hey</t>
-  </si>
-  <si>
     <t>Arabic Ligature Jallajalalouhou</t>
   </si>
   <si>
@@ -1207,13 +1186,91 @@
   </si>
   <si>
     <t>question</t>
+  </si>
+  <si>
+    <t>&amp;#FD3E</t>
+  </si>
+  <si>
+    <t>&amp;#FD3F</t>
+  </si>
+  <si>
+    <t>FDFC</t>
+  </si>
+  <si>
+    <t>Arabic Small High Lam Alef</t>
+  </si>
+  <si>
+    <t>&amp;#x6d9</t>
+  </si>
+  <si>
+    <t>Arabic Ligature Lam With Alef Isolated Form</t>
+  </si>
+  <si>
+    <t>&amp;#xfefb</t>
+  </si>
+  <si>
+    <t>Arabic Letter Heh Doachashmee</t>
+  </si>
+  <si>
+    <t>&amp;#x6be</t>
+  </si>
+  <si>
+    <t>&amp;#x603</t>
+  </si>
+  <si>
+    <t>Arabic Sign Safha</t>
+  </si>
+  <si>
+    <t>Arabic Ligature Salla Used As Koranic Stop Sign Isolated Form</t>
+  </si>
+  <si>
+    <t>&amp;#xfdf0</t>
+  </si>
+  <si>
+    <t>could not find high character</t>
+  </si>
+  <si>
+    <t>Dot Above</t>
+  </si>
+  <si>
+    <t>&amp;#x2d9</t>
+  </si>
+  <si>
+    <t>Number Comma</t>
+  </si>
+  <si>
+    <t>English Full Stop</t>
+  </si>
+  <si>
+    <t>Arabic Subscript Alef</t>
+  </si>
+  <si>
+    <t>&amp;#x656</t>
+  </si>
+  <si>
+    <t>Arabic Letter Lam</t>
+  </si>
+  <si>
+    <t>&amp;#x644</t>
+  </si>
+  <si>
+    <t>Arabic Jazam</t>
+  </si>
+  <si>
+    <t>Arabic Letter Yeh Isolated Form</t>
+  </si>
+  <si>
+    <t>&amp;#xfef1</t>
+  </si>
+  <si>
+    <t>PDF has a dot, unicode dose not</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1257,6 +1314,12 @@
       <sz val="12"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1306,7 +1369,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="67">
+  <cellStyleXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1374,8 +1437,96 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1411,8 +1562,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="67">
+  <cellStyles count="155">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1446,6 +1598,50 @@
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1479,6 +1675,50 @@
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1810,8 +2050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:KE201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="C190" sqref="C190"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="C191" sqref="C191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1819,20 +2059,21 @@
     <col min="1" max="1" width="19.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="52.6640625" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="10"/>
+    <col min="4" max="4" width="25.6640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="10"/>
     <col min="6" max="6" width="12" style="10" customWidth="1"/>
     <col min="7" max="291" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:291">
       <c r="A1" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:291">
@@ -1840,7 +2081,7 @@
     </row>
     <row r="3" spans="1:291">
       <c r="A3" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:291" s="10" customFormat="1">
@@ -1848,7 +2089,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -2468,21 +2709,21 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:291" s="3" customFormat="1">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>130</v>
+      <c r="C9" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -2773,15 +3014,15 @@
       <c r="KD9" s="10"/>
       <c r="KE9" s="10"/>
     </row>
-    <row r="10" spans="1:291">
-      <c r="A10" s="2">
+    <row r="10" spans="1:291" s="10" customFormat="1">
+      <c r="A10" s="8">
         <v>2</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>115</v>
+      <c r="B10" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:291" s="3" customFormat="1">
@@ -2789,10 +3030,10 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -3083,304 +3324,16 @@
       <c r="KD11" s="10"/>
       <c r="KE11" s="10"/>
     </row>
-    <row r="12" spans="1:291" s="3" customFormat="1">
-      <c r="A12" s="2">
+    <row r="12" spans="1:291" s="10" customFormat="1">
+      <c r="A12" s="8">
         <v>3</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="10"/>
-      <c r="Y12" s="10"/>
-      <c r="Z12" s="10"/>
-      <c r="AA12" s="10"/>
-      <c r="AB12" s="10"/>
-      <c r="AC12" s="10"/>
-      <c r="AD12" s="10"/>
-      <c r="AE12" s="10"/>
-      <c r="AF12" s="10"/>
-      <c r="AG12" s="10"/>
-      <c r="AH12" s="10"/>
-      <c r="AI12" s="10"/>
-      <c r="AJ12" s="10"/>
-      <c r="AK12" s="10"/>
-      <c r="AL12" s="10"/>
-      <c r="AM12" s="10"/>
-      <c r="AN12" s="10"/>
-      <c r="AO12" s="10"/>
-      <c r="AP12" s="10"/>
-      <c r="AQ12" s="10"/>
-      <c r="AR12" s="10"/>
-      <c r="AS12" s="10"/>
-      <c r="AT12" s="10"/>
-      <c r="AU12" s="10"/>
-      <c r="AV12" s="10"/>
-      <c r="AW12" s="10"/>
-      <c r="AX12" s="10"/>
-      <c r="AY12" s="10"/>
-      <c r="AZ12" s="10"/>
-      <c r="BA12" s="10"/>
-      <c r="BB12" s="10"/>
-      <c r="BC12" s="10"/>
-      <c r="BD12" s="10"/>
-      <c r="BE12" s="10"/>
-      <c r="BF12" s="10"/>
-      <c r="BG12" s="10"/>
-      <c r="BH12" s="10"/>
-      <c r="BI12" s="10"/>
-      <c r="BJ12" s="10"/>
-      <c r="BK12" s="10"/>
-      <c r="BL12" s="10"/>
-      <c r="BM12" s="10"/>
-      <c r="BN12" s="10"/>
-      <c r="BO12" s="10"/>
-      <c r="BP12" s="10"/>
-      <c r="BQ12" s="10"/>
-      <c r="BR12" s="10"/>
-      <c r="BS12" s="10"/>
-      <c r="BT12" s="10"/>
-      <c r="BU12" s="10"/>
-      <c r="BV12" s="10"/>
-      <c r="BW12" s="10"/>
-      <c r="BX12" s="10"/>
-      <c r="BY12" s="10"/>
-      <c r="BZ12" s="10"/>
-      <c r="CA12" s="10"/>
-      <c r="CB12" s="10"/>
-      <c r="CC12" s="10"/>
-      <c r="CD12" s="10"/>
-      <c r="CE12" s="10"/>
-      <c r="CF12" s="10"/>
-      <c r="CG12" s="10"/>
-      <c r="CH12" s="10"/>
-      <c r="CI12" s="10"/>
-      <c r="CJ12" s="10"/>
-      <c r="CK12" s="10"/>
-      <c r="CL12" s="10"/>
-      <c r="CM12" s="10"/>
-      <c r="CN12" s="10"/>
-      <c r="CO12" s="10"/>
-      <c r="CP12" s="10"/>
-      <c r="CQ12" s="10"/>
-      <c r="CR12" s="10"/>
-      <c r="CS12" s="10"/>
-      <c r="CT12" s="10"/>
-      <c r="CU12" s="10"/>
-      <c r="CV12" s="10"/>
-      <c r="CW12" s="10"/>
-      <c r="CX12" s="10"/>
-      <c r="CY12" s="10"/>
-      <c r="CZ12" s="10"/>
-      <c r="DA12" s="10"/>
-      <c r="DB12" s="10"/>
-      <c r="DC12" s="10"/>
-      <c r="DD12" s="10"/>
-      <c r="DE12" s="10"/>
-      <c r="DF12" s="10"/>
-      <c r="DG12" s="10"/>
-      <c r="DH12" s="10"/>
-      <c r="DI12" s="10"/>
-      <c r="DJ12" s="10"/>
-      <c r="DK12" s="10"/>
-      <c r="DL12" s="10"/>
-      <c r="DM12" s="10"/>
-      <c r="DN12" s="10"/>
-      <c r="DO12" s="10"/>
-      <c r="DP12" s="10"/>
-      <c r="DQ12" s="10"/>
-      <c r="DR12" s="10"/>
-      <c r="DS12" s="10"/>
-      <c r="DT12" s="10"/>
-      <c r="DU12" s="10"/>
-      <c r="DV12" s="10"/>
-      <c r="DW12" s="10"/>
-      <c r="DX12" s="10"/>
-      <c r="DY12" s="10"/>
-      <c r="DZ12" s="10"/>
-      <c r="EA12" s="10"/>
-      <c r="EB12" s="10"/>
-      <c r="EC12" s="10"/>
-      <c r="ED12" s="10"/>
-      <c r="EE12" s="10"/>
-      <c r="EF12" s="10"/>
-      <c r="EG12" s="10"/>
-      <c r="EH12" s="10"/>
-      <c r="EI12" s="10"/>
-      <c r="EJ12" s="10"/>
-      <c r="EK12" s="10"/>
-      <c r="EL12" s="10"/>
-      <c r="EM12" s="10"/>
-      <c r="EN12" s="10"/>
-      <c r="EO12" s="10"/>
-      <c r="EP12" s="10"/>
-      <c r="EQ12" s="10"/>
-      <c r="ER12" s="10"/>
-      <c r="ES12" s="10"/>
-      <c r="ET12" s="10"/>
-      <c r="EU12" s="10"/>
-      <c r="EV12" s="10"/>
-      <c r="EW12" s="10"/>
-      <c r="EX12" s="10"/>
-      <c r="EY12" s="10"/>
-      <c r="EZ12" s="10"/>
-      <c r="FA12" s="10"/>
-      <c r="FB12" s="10"/>
-      <c r="FC12" s="10"/>
-      <c r="FD12" s="10"/>
-      <c r="FE12" s="10"/>
-      <c r="FF12" s="10"/>
-      <c r="FG12" s="10"/>
-      <c r="FH12" s="10"/>
-      <c r="FI12" s="10"/>
-      <c r="FJ12" s="10"/>
-      <c r="FK12" s="10"/>
-      <c r="FL12" s="10"/>
-      <c r="FM12" s="10"/>
-      <c r="FN12" s="10"/>
-      <c r="FO12" s="10"/>
-      <c r="FP12" s="10"/>
-      <c r="FQ12" s="10"/>
-      <c r="FR12" s="10"/>
-      <c r="FS12" s="10"/>
-      <c r="FT12" s="10"/>
-      <c r="FU12" s="10"/>
-      <c r="FV12" s="10"/>
-      <c r="FW12" s="10"/>
-      <c r="FX12" s="10"/>
-      <c r="FY12" s="10"/>
-      <c r="FZ12" s="10"/>
-      <c r="GA12" s="10"/>
-      <c r="GB12" s="10"/>
-      <c r="GC12" s="10"/>
-      <c r="GD12" s="10"/>
-      <c r="GE12" s="10"/>
-      <c r="GF12" s="10"/>
-      <c r="GG12" s="10"/>
-      <c r="GH12" s="10"/>
-      <c r="GI12" s="10"/>
-      <c r="GJ12" s="10"/>
-      <c r="GK12" s="10"/>
-      <c r="GL12" s="10"/>
-      <c r="GM12" s="10"/>
-      <c r="GN12" s="10"/>
-      <c r="GO12" s="10"/>
-      <c r="GP12" s="10"/>
-      <c r="GQ12" s="10"/>
-      <c r="GR12" s="10"/>
-      <c r="GS12" s="10"/>
-      <c r="GT12" s="10"/>
-      <c r="GU12" s="10"/>
-      <c r="GV12" s="10"/>
-      <c r="GW12" s="10"/>
-      <c r="GX12" s="10"/>
-      <c r="GY12" s="10"/>
-      <c r="GZ12" s="10"/>
-      <c r="HA12" s="10"/>
-      <c r="HB12" s="10"/>
-      <c r="HC12" s="10"/>
-      <c r="HD12" s="10"/>
-      <c r="HE12" s="10"/>
-      <c r="HF12" s="10"/>
-      <c r="HG12" s="10"/>
-      <c r="HH12" s="10"/>
-      <c r="HI12" s="10"/>
-      <c r="HJ12" s="10"/>
-      <c r="HK12" s="10"/>
-      <c r="HL12" s="10"/>
-      <c r="HM12" s="10"/>
-      <c r="HN12" s="10"/>
-      <c r="HO12" s="10"/>
-      <c r="HP12" s="10"/>
-      <c r="HQ12" s="10"/>
-      <c r="HR12" s="10"/>
-      <c r="HS12" s="10"/>
-      <c r="HT12" s="10"/>
-      <c r="HU12" s="10"/>
-      <c r="HV12" s="10"/>
-      <c r="HW12" s="10"/>
-      <c r="HX12" s="10"/>
-      <c r="HY12" s="10"/>
-      <c r="HZ12" s="10"/>
-      <c r="IA12" s="10"/>
-      <c r="IB12" s="10"/>
-      <c r="IC12" s="10"/>
-      <c r="ID12" s="10"/>
-      <c r="IE12" s="10"/>
-      <c r="IF12" s="10"/>
-      <c r="IG12" s="10"/>
-      <c r="IH12" s="10"/>
-      <c r="II12" s="10"/>
-      <c r="IJ12" s="10"/>
-      <c r="IK12" s="10"/>
-      <c r="IL12" s="10"/>
-      <c r="IM12" s="10"/>
-      <c r="IN12" s="10"/>
-      <c r="IO12" s="10"/>
-      <c r="IP12" s="10"/>
-      <c r="IQ12" s="10"/>
-      <c r="IR12" s="10"/>
-      <c r="IS12" s="10"/>
-      <c r="IT12" s="10"/>
-      <c r="IU12" s="10"/>
-      <c r="IV12" s="10"/>
-      <c r="IW12" s="10"/>
-      <c r="IX12" s="10"/>
-      <c r="IY12" s="10"/>
-      <c r="IZ12" s="10"/>
-      <c r="JA12" s="10"/>
-      <c r="JB12" s="10"/>
-      <c r="JC12" s="10"/>
-      <c r="JD12" s="10"/>
-      <c r="JE12" s="10"/>
-      <c r="JF12" s="10"/>
-      <c r="JG12" s="10"/>
-      <c r="JH12" s="10"/>
-      <c r="JI12" s="10"/>
-      <c r="JJ12" s="10"/>
-      <c r="JK12" s="10"/>
-      <c r="JL12" s="10"/>
-      <c r="JM12" s="10"/>
-      <c r="JN12" s="10"/>
-      <c r="JO12" s="10"/>
-      <c r="JP12" s="10"/>
-      <c r="JQ12" s="10"/>
-      <c r="JR12" s="10"/>
-      <c r="JS12" s="10"/>
-      <c r="JT12" s="10"/>
-      <c r="JU12" s="10"/>
-      <c r="JV12" s="10"/>
-      <c r="JW12" s="10"/>
-      <c r="JX12" s="10"/>
-      <c r="JY12" s="10"/>
-      <c r="JZ12" s="10"/>
-      <c r="KA12" s="10"/>
-      <c r="KB12" s="10"/>
-      <c r="KC12" s="10"/>
-      <c r="KD12" s="10"/>
-      <c r="KE12" s="10"/>
+      <c r="B12" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="13" spans="1:291" s="3" customFormat="1">
       <c r="A13" s="1" t="s">
@@ -3686,10 +3639,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:291" s="3" customFormat="1">
@@ -3697,10 +3650,10 @@
         <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>102</v>
+        <v>413</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>101</v>
+        <v>412</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -3991,15 +3944,15 @@
       <c r="KD15" s="10"/>
       <c r="KE15" s="10"/>
     </row>
-    <row r="16" spans="1:291">
-      <c r="A16" s="2">
+    <row r="16" spans="1:291" s="10" customFormat="1">
+      <c r="A16" s="8">
         <v>5</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>118</v>
+      <c r="B16" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:291" s="3" customFormat="1">
@@ -4007,10 +3960,10 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -4306,10 +4259,10 @@
         <v>6</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:291" s="3" customFormat="1">
@@ -4317,10 +4270,10 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -4616,10 +4569,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:291" s="3" customFormat="1">
@@ -4627,10 +4580,10 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -4921,15 +4874,15 @@
       <c r="KD21" s="10"/>
       <c r="KE21" s="10"/>
     </row>
-    <row r="22" spans="1:291">
-      <c r="A22" s="2">
+    <row r="22" spans="1:291" s="10" customFormat="1">
+      <c r="A22" s="8">
         <v>8</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>121</v>
+      <c r="B22" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:291" s="3" customFormat="1">
@@ -4940,7 +4893,7 @@
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -5231,15 +5184,15 @@
       <c r="KD23" s="10"/>
       <c r="KE23" s="10"/>
     </row>
-    <row r="24" spans="1:291">
-      <c r="A24" s="2">
+    <row r="24" spans="1:291" s="10" customFormat="1">
+      <c r="A24" s="8">
         <v>9</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>122</v>
+      <c r="B24" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:291">
@@ -5250,18 +5203,18 @@
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:291">
-      <c r="A26" s="2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:291" s="10" customFormat="1">
+      <c r="A26" s="8">
         <v>0</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>112</v>
+      <c r="B26" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:291">
@@ -5269,10 +5222,10 @@
         <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:291">
@@ -5280,10 +5233,10 @@
         <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:291">
@@ -5291,10 +5244,10 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C29" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:291" s="5" customFormat="1">
@@ -5302,10 +5255,10 @@
         <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C30" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
@@ -5601,10 +5554,10 @@
         <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C31" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:291">
@@ -5612,10 +5565,10 @@
         <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C32" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:291">
@@ -5624,7 +5577,7 @@
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:291" s="5" customFormat="1">
@@ -5632,10 +5585,10 @@
         <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -5931,10 +5884,10 @@
         <v>22</v>
       </c>
       <c r="B35" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:291">
@@ -5942,10 +5895,10 @@
         <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C36" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:291">
@@ -5954,7 +5907,7 @@
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:291">
@@ -5962,10 +5915,10 @@
         <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:291">
@@ -5973,10 +5926,10 @@
         <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C39" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:291" s="3" customFormat="1">
@@ -5984,10 +5937,10 @@
         <v>27</v>
       </c>
       <c r="B40" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
@@ -6283,10 +6236,10 @@
         <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:291">
@@ -6294,10 +6247,10 @@
         <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C42" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:291">
@@ -6305,10 +6258,13 @@
         <v>30</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="44" spans="1:291" s="3" customFormat="1">
@@ -6316,10 +6272,10 @@
         <v>31</v>
       </c>
       <c r="B44" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C44" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
@@ -6615,10 +6571,10 @@
         <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C45" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:291">
@@ -6626,10 +6582,10 @@
         <v>33</v>
       </c>
       <c r="B46" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C46" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:291">
@@ -6637,10 +6593,10 @@
         <v>34</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:291">
@@ -6648,10 +6604,10 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C48" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:291">
@@ -6659,10 +6615,10 @@
         <v>36</v>
       </c>
       <c r="B49" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C49" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:291" s="6" customFormat="1">
@@ -6670,10 +6626,10 @@
         <v>37</v>
       </c>
       <c r="B50" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C50" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
@@ -6969,10 +6925,10 @@
         <v>38</v>
       </c>
       <c r="B51" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C51" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:291" s="6" customFormat="1">
@@ -6980,10 +6936,10 @@
         <v>39</v>
       </c>
       <c r="B52" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C52" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
@@ -7293,7 +7249,7 @@
         <v>41</v>
       </c>
       <c r="C54" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="55" spans="1:291">
@@ -7315,7 +7271,7 @@
         <v>43</v>
       </c>
       <c r="C56" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:291">
@@ -7323,10 +7279,10 @@
         <v>44</v>
       </c>
       <c r="B57" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C57" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:291">
@@ -7345,10 +7301,10 @@
         <v>46</v>
       </c>
       <c r="B59" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C59" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="60" spans="1:291" s="5" customFormat="1">
@@ -7356,10 +7312,10 @@
         <v>47</v>
       </c>
       <c r="B60" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C60" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D60" s="10"/>
       <c r="E60" s="10"/>
@@ -7655,10 +7611,10 @@
         <v>48</v>
       </c>
       <c r="B61" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C61" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:291">
@@ -7666,28 +7622,32 @@
         <v>49</v>
       </c>
       <c r="B62" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C62" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="63" spans="1:291">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
+      <c r="B63" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="64" spans="1:291">
       <c r="A64" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C64" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:291" s="5" customFormat="1">
@@ -7695,10 +7655,10 @@
         <v>52</v>
       </c>
       <c r="B65" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C65" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D65" s="10"/>
       <c r="E65" s="10"/>
@@ -7994,10 +7954,10 @@
         <v>53</v>
       </c>
       <c r="B66" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C66" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67" spans="1:291">
@@ -8005,28 +7965,32 @@
         <v>54</v>
       </c>
       <c r="B67" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C67" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:291">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
+      <c r="B68" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="69" spans="1:291">
       <c r="A69" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B69" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C69" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="70" spans="1:291" s="5" customFormat="1">
@@ -8034,10 +7998,10 @@
         <v>57</v>
       </c>
       <c r="B70" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C70" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D70" s="10"/>
       <c r="E70" s="10"/>
@@ -8333,10 +8297,10 @@
         <v>58</v>
       </c>
       <c r="B71" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C71" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71" s="10"/>
@@ -8632,10 +8596,10 @@
         <v>59</v>
       </c>
       <c r="B72" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C72" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="73" spans="1:291">
@@ -8644,16 +8608,18 @@
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="74" spans="1:291">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5" t="s">
-        <v>208</v>
+      <c r="B74" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="75" spans="1:291" s="3" customFormat="1">
@@ -8664,7 +8630,7 @@
         <v>62</v>
       </c>
       <c r="C75" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D75" s="10"/>
       <c r="E75" s="10"/>
@@ -8960,10 +8926,10 @@
         <v>63</v>
       </c>
       <c r="B76" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C76" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="77" spans="1:291">
@@ -8971,10 +8937,10 @@
         <v>64</v>
       </c>
       <c r="B77" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C77" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="78" spans="1:291">
@@ -8982,10 +8948,10 @@
         <v>65</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="79" spans="1:291">
@@ -8993,10 +8959,10 @@
         <v>67</v>
       </c>
       <c r="B79" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C79" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="80" spans="1:291">
@@ -9004,10 +8970,10 @@
         <v>66</v>
       </c>
       <c r="B80" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C80" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="81" spans="1:291">
@@ -9015,10 +8981,10 @@
         <v>68</v>
       </c>
       <c r="B81" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C81" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="82" spans="1:291">
@@ -9026,10 +8992,10 @@
         <v>69</v>
       </c>
       <c r="B82" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C82" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="83" spans="1:291">
@@ -9037,10 +9003,10 @@
         <v>70</v>
       </c>
       <c r="B83" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C83" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="84" spans="1:291" s="5" customFormat="1">
@@ -9048,10 +9014,10 @@
         <v>71</v>
       </c>
       <c r="B84" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C84" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D84" s="10"/>
       <c r="E84" s="10"/>
@@ -9347,10 +9313,10 @@
         <v>72</v>
       </c>
       <c r="B85" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C85" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="86" spans="1:291">
@@ -9358,10 +9324,10 @@
         <v>73</v>
       </c>
       <c r="B86" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C86" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="87" spans="1:291">
@@ -9370,7 +9336,7 @@
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="88" spans="1:291">
@@ -9378,10 +9344,10 @@
         <v>75</v>
       </c>
       <c r="B88" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C88" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="89" spans="1:291">
@@ -9389,10 +9355,10 @@
         <v>76</v>
       </c>
       <c r="B89" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C89" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="90" spans="1:291">
@@ -9400,10 +9366,10 @@
         <v>77</v>
       </c>
       <c r="B90" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C90" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="91" spans="1:291">
@@ -9411,10 +9377,10 @@
         <v>78</v>
       </c>
       <c r="B91" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C91" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="92" spans="1:291">
@@ -9422,10 +9388,10 @@
         <v>79</v>
       </c>
       <c r="B92" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C92" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="93" spans="1:291" s="5" customFormat="1">
@@ -9433,10 +9399,10 @@
         <v>80</v>
       </c>
       <c r="B93" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C93" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D93" s="10"/>
       <c r="E93" s="10"/>
@@ -9743,10 +9709,10 @@
         <v>82</v>
       </c>
       <c r="B95" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C95" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D95" s="10"/>
       <c r="E95" s="10"/>
@@ -10043,7 +10009,7 @@
       </c>
       <c r="B96" s="5"/>
       <c r="C96" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -10062,11 +10028,13 @@
         <v>85</v>
       </c>
       <c r="B98" s="5"/>
-      <c r="C98" s="5"/>
+      <c r="C98" s="5" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="8" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -10074,10 +10042,10 @@
         <v>2</v>
       </c>
       <c r="B101" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C101" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -10085,10 +10053,10 @@
         <v>3</v>
       </c>
       <c r="B102" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C102" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -10096,10 +10064,10 @@
         <v>4</v>
       </c>
       <c r="B103" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C103" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -10107,10 +10075,10 @@
         <v>1</v>
       </c>
       <c r="B104" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C104" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -10121,7 +10089,7 @@
         <v>5</v>
       </c>
       <c r="C105" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -10129,10 +10097,10 @@
         <v>2</v>
       </c>
       <c r="B106" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C106" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -10143,7 +10111,7 @@
         <v>6</v>
       </c>
       <c r="C107" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -10151,10 +10119,10 @@
         <v>3</v>
       </c>
       <c r="B108" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -10165,7 +10133,7 @@
         <v>7</v>
       </c>
       <c r="C109" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -10173,10 +10141,10 @@
         <v>4</v>
       </c>
       <c r="B110" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -10187,7 +10155,7 @@
         <v>8</v>
       </c>
       <c r="C111" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -10195,10 +10163,10 @@
         <v>5</v>
       </c>
       <c r="B112" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -10209,7 +10177,7 @@
         <v>9</v>
       </c>
       <c r="C113" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -10217,10 +10185,10 @@
         <v>6</v>
       </c>
       <c r="B114" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C114" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -10231,7 +10199,7 @@
         <v>10</v>
       </c>
       <c r="C115" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -10239,10 +10207,10 @@
         <v>7</v>
       </c>
       <c r="B116" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C116" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -10253,7 +10221,7 @@
         <v>11</v>
       </c>
       <c r="C117" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -10261,10 +10229,10 @@
         <v>8</v>
       </c>
       <c r="B118" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C118" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -10272,10 +10240,10 @@
         <v>12</v>
       </c>
       <c r="B119" s="15" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -10283,10 +10251,10 @@
         <v>9</v>
       </c>
       <c r="B120" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C120" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -10295,7 +10263,7 @@
       </c>
       <c r="B121" s="17"/>
       <c r="C121" s="17" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -10303,10 +10271,10 @@
         <v>0</v>
       </c>
       <c r="B122" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C122" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -10317,7 +10285,7 @@
         <v>14</v>
       </c>
       <c r="C123" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -10328,7 +10296,7 @@
         <v>15</v>
       </c>
       <c r="C124" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -10339,7 +10307,7 @@
         <v>16</v>
       </c>
       <c r="C125" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -10350,7 +10318,7 @@
         <v>17</v>
       </c>
       <c r="C126" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -10361,7 +10329,7 @@
         <v>19</v>
       </c>
       <c r="C127" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -10369,154 +10337,156 @@
         <v>19</v>
       </c>
       <c r="B128" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C128" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B129" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C129" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B130" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C130" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B131" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C131" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B132" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C132" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" s="10" customFormat="1">
-      <c r="A133" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" s="10" customFormat="1">
+      <c r="A133" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B133" s="5"/>
-      <c r="C133" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3">
+      <c r="B133" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="C133" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B134" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C134" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B135" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C135" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B136" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C136" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B137" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C137" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B138" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C138" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
       <c r="A139" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B139" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C139" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B140" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C140" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B141" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C141" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142" s="8" t="s">
         <v>33</v>
       </c>
@@ -10527,22 +10497,30 @@
         <v>98</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
-      <c r="A143" s="4" t="s">
+    <row r="143" spans="1:4">
+      <c r="A143" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B143" s="5"/>
-      <c r="C143" s="5" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3">
+      <c r="B143" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="D143" s="10" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B144" s="5"/>
       <c r="C144" s="5" t="s">
-        <v>321</v>
+        <v>316</v>
+      </c>
+      <c r="D144" s="10" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -10550,10 +10528,10 @@
         <v>36</v>
       </c>
       <c r="B145" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C145" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -10561,10 +10539,10 @@
         <v>37</v>
       </c>
       <c r="B146" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C146" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -10572,10 +10550,10 @@
         <v>38</v>
       </c>
       <c r="B147" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C147" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -10583,10 +10561,10 @@
         <v>39</v>
       </c>
       <c r="B148" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C148" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -10597,16 +10575,18 @@
         <v>40</v>
       </c>
       <c r="C149" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="150" spans="1:3">
-      <c r="A150" s="4" t="s">
+      <c r="A150" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B150" s="5"/>
-      <c r="C150" s="5" t="s">
-        <v>332</v>
+      <c r="B150" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="C150" s="10" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -10617,16 +10597,18 @@
         <v>42</v>
       </c>
       <c r="C151" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="152" spans="1:3">
-      <c r="A152" s="4" t="s">
+      <c r="A152" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B152" s="5"/>
-      <c r="C152" s="5" t="s">
-        <v>333</v>
+      <c r="B152" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="C152" s="10" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -10634,10 +10616,10 @@
         <v>44</v>
       </c>
       <c r="B153" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C153" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -10645,10 +10627,10 @@
         <v>45</v>
       </c>
       <c r="B154" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C154" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -10656,19 +10638,21 @@
         <v>46</v>
       </c>
       <c r="B155" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C155" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="156" spans="1:3" s="10" customFormat="1">
-      <c r="A156" s="4" t="s">
+      <c r="A156" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B156" s="5"/>
-      <c r="C156" s="5" t="s">
-        <v>340</v>
+      <c r="B156" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="C156" s="10" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -10676,10 +10660,10 @@
         <v>48</v>
       </c>
       <c r="B157" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C157" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -10687,10 +10671,10 @@
         <v>49</v>
       </c>
       <c r="B158" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C158" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -10698,10 +10682,10 @@
         <v>50</v>
       </c>
       <c r="B159" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C159" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -10709,10 +10693,10 @@
         <v>51</v>
       </c>
       <c r="B160" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C160" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -10720,10 +10704,10 @@
         <v>52</v>
       </c>
       <c r="B161" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C161" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -10731,10 +10715,10 @@
         <v>53</v>
       </c>
       <c r="B162" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C162" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -10742,19 +10726,21 @@
         <v>54</v>
       </c>
       <c r="B163" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C163" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="164" spans="1:3">
-      <c r="A164" s="4" t="s">
+      <c r="A164" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B164" s="5"/>
-      <c r="C164" s="5" t="s">
-        <v>357</v>
+      <c r="B164" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="C164" s="10" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -10762,10 +10748,10 @@
         <v>56</v>
       </c>
       <c r="B165" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C165" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -10773,10 +10759,10 @@
         <v>57</v>
       </c>
       <c r="B166" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="C166" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -10784,10 +10770,10 @@
         <v>58</v>
       </c>
       <c r="B167" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C167" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -10795,35 +10781,43 @@
         <v>59</v>
       </c>
       <c r="B168" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="C168" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="169" spans="1:3">
-      <c r="A169" s="4" t="s">
+      <c r="A169" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B169" s="5"/>
-      <c r="C169" s="5"/>
+      <c r="B169" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="C169" s="10" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="170" spans="1:3">
-      <c r="A170" s="4" t="s">
+      <c r="A170" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B170" s="5"/>
-      <c r="C170" s="5"/>
+      <c r="B170" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="C170" s="10" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="8" t="s">
         <v>62</v>
       </c>
       <c r="B171" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C171" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -10834,7 +10828,7 @@
         <v>63</v>
       </c>
       <c r="C172" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -10845,7 +10839,7 @@
         <v>64</v>
       </c>
       <c r="C173" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -10856,7 +10850,7 @@
         <v>65</v>
       </c>
       <c r="C174" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -10864,10 +10858,10 @@
         <v>67</v>
       </c>
       <c r="B175" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="C175" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -10875,10 +10869,10 @@
         <v>66</v>
       </c>
       <c r="B176" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="C176" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -10886,10 +10880,10 @@
         <v>68</v>
       </c>
       <c r="B177" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="C177" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -10897,10 +10891,10 @@
         <v>69</v>
       </c>
       <c r="B178" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="C178" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -10908,10 +10902,10 @@
         <v>70</v>
       </c>
       <c r="B179" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C179" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -10919,19 +10913,21 @@
         <v>71</v>
       </c>
       <c r="B180" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="C180" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="181" spans="1:3">
-      <c r="A181" s="4" t="s">
+      <c r="A181" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B181" s="5"/>
-      <c r="C181" s="5" t="s">
-        <v>377</v>
+      <c r="B181" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="C181" s="10" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -10939,10 +10935,10 @@
         <v>73</v>
       </c>
       <c r="B182" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="C182" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -10950,10 +10946,10 @@
         <v>74</v>
       </c>
       <c r="B183" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="C183" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -10961,10 +10957,10 @@
         <v>75</v>
       </c>
       <c r="B184" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C184" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -10972,10 +10968,10 @@
         <v>76</v>
       </c>
       <c r="B185" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C185" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -10983,10 +10979,10 @@
         <v>77</v>
       </c>
       <c r="B186" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="C186" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -10994,10 +10990,10 @@
         <v>78</v>
       </c>
       <c r="B187" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="C187" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="188" spans="1:3" s="10" customFormat="1">
@@ -11005,10 +11001,10 @@
         <v>79</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -11019,15 +11015,17 @@
         <v>80</v>
       </c>
       <c r="C189" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
     </row>
     <row r="190" spans="1:3">
-      <c r="A190" s="2" t="s">
+      <c r="A190" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B190" s="3"/>
-      <c r="C190" s="3"/>
+      <c r="B190" s="13"/>
+      <c r="C190" s="13" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="8" t="s">
@@ -11037,15 +11035,17 @@
         <v>84</v>
       </c>
       <c r="C191" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="192" spans="1:3">
-      <c r="A192" s="2" t="s">
+      <c r="A192" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B192" s="3"/>
-      <c r="C192" s="3"/>
+      <c r="B192" s="13"/>
+      <c r="C192" s="13" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="8" t="s">
@@ -11055,7 +11055,7 @@
         <v>84</v>
       </c>
       <c r="C193" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -11066,7 +11066,7 @@
         <v>85</v>
       </c>
       <c r="C194" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="195" spans="1:3">

</xml_diff>

<commit_message>
Modifying some of the keys and implementing much of the main and shift 5 row key values
</commit_message>
<xml_diff>
--- a/Resources/TranslationKeys.xlsx
+++ b/Resources/TranslationKeys.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-440" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="-80" yWindow="0" windowWidth="12800" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="420">
   <si>
     <t>Arabic Name</t>
   </si>
@@ -1264,6 +1264,21 @@
   </si>
   <si>
     <t>PDF has a dot, unicode dose not</t>
+  </si>
+  <si>
+    <t>Arabic Letter Alef With Madda Above</t>
+  </si>
+  <si>
+    <t>&amp;#x622;</t>
+  </si>
+  <si>
+    <t>&amp;#x60e;</t>
+  </si>
+  <si>
+    <t>&amp;#x621;</t>
+  </si>
+  <si>
+    <t>&amp;#x62d</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1384,388 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="155">
+  <cellStyleXfs count="535">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1564,7 +1959,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="155">
+  <cellStyles count="535">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1642,6 +2037,196 @@
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="482" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="484" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="486" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="488" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="490" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="492" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="494" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="496" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="498" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="500" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="502" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="504" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="506" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="520" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="522" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="524" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="526" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="528" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="530" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="532" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="534" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1719,6 +2304,196 @@
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="481" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="483" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="485" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="489" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="491" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="493" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="495" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="497" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="499" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="501" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="503" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="519" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="521" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="523" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="525" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="527" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="529" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="531" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="533" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2048,10 +2823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:KE201"/>
+  <dimension ref="A1:KE206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="C191" sqref="C191"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3340,10 +4115,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>418</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>170</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -5244,10 +6019,10 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>139</v>
+        <v>416</v>
       </c>
       <c r="C29" t="s">
-        <v>140</v>
+        <v>415</v>
       </c>
     </row>
     <row r="30" spans="1:291" s="5" customFormat="1">
@@ -5571,24 +6346,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:291">
-      <c r="A33" s="4" t="s">
+    <row r="34" spans="1:291" s="5" customFormat="1">
+      <c r="A34" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="34" spans="1:291" s="5" customFormat="1">
-      <c r="A34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" t="s">
-        <v>107</v>
-      </c>
-      <c r="C34" t="s">
-        <v>108</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -5881,66 +6644,66 @@
     </row>
     <row r="35" spans="1:291">
       <c r="A35" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="C35" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:291">
       <c r="A36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>149</v>
+      </c>
+      <c r="C36" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:291">
+      <c r="A37" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>151</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="37" spans="1:291">
-      <c r="A37" s="4" t="s">
+    <row r="38" spans="1:291">
+      <c r="A38" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5" t="s">
+      <c r="B38" s="5"/>
+      <c r="C38" s="5" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="38" spans="1:291">
-      <c r="A38" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B38" t="s">
-        <v>154</v>
-      </c>
-      <c r="C38" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:291">
       <c r="A39" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C39" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:291" s="3" customFormat="1">
       <c r="A40" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B40" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C40" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
@@ -6233,49 +6996,49 @@
     </row>
     <row r="41" spans="1:291">
       <c r="A41" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B41" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:291">
       <c r="A42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" t="s">
+        <v>160</v>
+      </c>
+      <c r="C42" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:291">
+      <c r="A43" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>161</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="43" spans="1:291">
-      <c r="A43" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="44" spans="1:291" s="3" customFormat="1">
-      <c r="A44" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44" t="s">
-        <v>166</v>
-      </c>
-      <c r="C44" t="s">
-        <v>165</v>
+      <c r="A44" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
@@ -6568,68 +7331,68 @@
     </row>
     <row r="45" spans="1:291">
       <c r="A45" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C45" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:291">
       <c r="A46" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" t="s">
+        <v>168</v>
+      </c>
+      <c r="C46" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:291">
+      <c r="A47" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>169</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:291">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:291">
+      <c r="A48" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="48" spans="1:291">
-      <c r="A48" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B48" t="s">
-        <v>104</v>
-      </c>
-      <c r="C48" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:291">
       <c r="A49" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>174</v>
+        <v>104</v>
       </c>
       <c r="C49" t="s">
-        <v>173</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:291" s="6" customFormat="1">
       <c r="A50" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B50" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C50" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
@@ -6922,24 +7685,24 @@
     </row>
     <row r="51" spans="1:291">
       <c r="A51" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C51" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="52" spans="1:291" s="6" customFormat="1">
       <c r="A52" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B52" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C52" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
@@ -7231,92 +7994,86 @@
       <c r="KE52" s="10"/>
     </row>
     <row r="53" spans="1:291">
-      <c r="A53" s="12" t="s">
+      <c r="A53" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53" t="s">
+        <v>180</v>
+      </c>
+      <c r="C53" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="54" spans="1:291">
+      <c r="A54" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="B54" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C54" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:291">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:291">
+      <c r="A55" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>41</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="55" spans="1:291">
-      <c r="A55" s="12" t="s">
+    <row r="56" spans="1:291">
+      <c r="A56" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B55" s="13" t="s">
+      <c r="B56" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C56" s="13" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="1:291">
-      <c r="A56" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B56" t="s">
-        <v>43</v>
-      </c>
-      <c r="C56" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:291">
       <c r="A57" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B57" t="s">
-        <v>184</v>
+        <v>43</v>
       </c>
       <c r="C57" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="58" spans="1:291">
       <c r="A58" s="1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B58" t="s">
-        <v>95</v>
+        <v>144</v>
       </c>
       <c r="C58" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" spans="1:291">
       <c r="A59" s="1" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="B59" t="s">
-        <v>185</v>
+        <v>417</v>
       </c>
       <c r="C59" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:291" s="5" customFormat="1">
-      <c r="A60" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B60" t="s">
-        <v>188</v>
-      </c>
-      <c r="C60" t="s">
-        <v>187</v>
-      </c>
+      <c r="A60" s="1"/>
+      <c r="B60"/>
+      <c r="C60"/>
       <c r="D60" s="10"/>
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
@@ -7608,57 +8365,57 @@
     </row>
     <row r="61" spans="1:291">
       <c r="A61" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B61" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C61" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="1:291">
       <c r="A62" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B62" t="s">
-        <v>191</v>
+        <v>95</v>
       </c>
       <c r="C62" t="s">
-        <v>192</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:291">
-      <c r="A63" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>408</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>407</v>
+      <c r="A63" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B63" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:291">
       <c r="A64" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B64" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C64" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="65" spans="1:291" s="5" customFormat="1">
       <c r="A65" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B65" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C65" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="D65" s="10"/>
       <c r="E65" s="10"/>
@@ -7951,57 +8708,57 @@
     </row>
     <row r="66" spans="1:291">
       <c r="A66" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B66" t="s">
-        <v>101</v>
+        <v>191</v>
       </c>
       <c r="C66" t="s">
-        <v>102</v>
+        <v>192</v>
       </c>
     </row>
     <row r="67" spans="1:291">
-      <c r="A67" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B67" t="s">
-        <v>101</v>
-      </c>
-      <c r="C67" t="s">
-        <v>102</v>
+      <c r="A67" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="68" spans="1:291">
-      <c r="A68" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>396</v>
+      <c r="A68" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B68" t="s">
+        <v>194</v>
+      </c>
+      <c r="C68" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="69" spans="1:291">
       <c r="A69" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B69" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C69" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="70" spans="1:291" s="5" customFormat="1">
       <c r="A70" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B70" t="s">
-        <v>199</v>
+        <v>101</v>
       </c>
       <c r="C70" t="s">
-        <v>200</v>
+        <v>102</v>
       </c>
       <c r="D70" s="10"/>
       <c r="E70" s="10"/>
@@ -8294,13 +9051,13 @@
     </row>
     <row r="71" spans="1:291" s="5" customFormat="1">
       <c r="A71" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B71" t="s">
-        <v>202</v>
+        <v>419</v>
       </c>
       <c r="C71" t="s">
-        <v>201</v>
+        <v>102</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71" s="10"/>
@@ -8592,45 +9349,47 @@
       <c r="KE71" s="10"/>
     </row>
     <row r="72" spans="1:291">
-      <c r="A72" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B72" t="s">
-        <v>204</v>
-      </c>
-      <c r="C72" t="s">
-        <v>203</v>
+      <c r="A72" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="73" spans="1:291">
-      <c r="A73" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5" t="s">
-        <v>205</v>
+      <c r="A73" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B73" t="s">
+        <v>198</v>
+      </c>
+      <c r="C73" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="1:291">
-      <c r="A74" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B74" s="10" t="s">
-        <v>410</v>
-      </c>
-      <c r="C74" s="10" t="s">
-        <v>409</v>
+      <c r="A74" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B74" t="s">
+        <v>199</v>
+      </c>
+      <c r="C74" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="75" spans="1:291" s="3" customFormat="1">
       <c r="A75" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B75" t="s">
-        <v>62</v>
+        <v>202</v>
       </c>
       <c r="C75" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D75" s="10"/>
       <c r="E75" s="10"/>
@@ -8923,101 +9682,93 @@
     </row>
     <row r="76" spans="1:291">
       <c r="A76" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B76" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C76" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="77" spans="1:291">
-      <c r="A77" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B77" t="s">
-        <v>209</v>
-      </c>
-      <c r="C77" t="s">
-        <v>210</v>
+      <c r="A77" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="78" spans="1:291">
-      <c r="A78" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>212</v>
+      <c r="A78" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="79" spans="1:291">
       <c r="A79" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B79" t="s">
-        <v>214</v>
+        <v>62</v>
       </c>
       <c r="C79" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="80" spans="1:291">
       <c r="A80" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B80" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C80" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="81" spans="1:291">
       <c r="A81" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B81" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C81" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="82" spans="1:291">
-      <c r="A82" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B82" t="s">
-        <v>219</v>
-      </c>
-      <c r="C82" t="s">
-        <v>220</v>
+      <c r="A82" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="83" spans="1:291">
-      <c r="A83" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B83" t="s">
-        <v>221</v>
-      </c>
-      <c r="C83" t="s">
-        <v>222</v>
-      </c>
+      <c r="A83" s="7"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
     </row>
     <row r="84" spans="1:291" s="5" customFormat="1">
       <c r="A84" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B84" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C84" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="D84" s="10"/>
       <c r="E84" s="10"/>
@@ -9310,99 +10061,99 @@
     </row>
     <row r="85" spans="1:291">
       <c r="A85" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B85" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C85" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
     <row r="86" spans="1:291">
       <c r="A86" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B86" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C86" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
     </row>
     <row r="87" spans="1:291">
-      <c r="A87" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B87" s="5"/>
-      <c r="C87" s="5" t="s">
-        <v>230</v>
+      <c r="A87" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B87" t="s">
+        <v>219</v>
+      </c>
+      <c r="C87" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="88" spans="1:291">
       <c r="A88" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B88" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="C88" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="1:291">
       <c r="A89" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B89" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C89" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
     </row>
     <row r="90" spans="1:291">
       <c r="A90" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B90" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C90" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="91" spans="1:291">
       <c r="A91" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B91" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="C91" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="92" spans="1:291">
-      <c r="A92" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B92" t="s">
-        <v>240</v>
-      </c>
-      <c r="C92" t="s">
-        <v>239</v>
+      <c r="A92" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="93" spans="1:291" s="5" customFormat="1">
       <c r="A93" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B93" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C93" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="D93" s="10"/>
       <c r="E93" s="10"/>
@@ -9695,24 +10446,24 @@
     </row>
     <row r="94" spans="1:291">
       <c r="A94" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B94" t="s">
-        <v>91</v>
+        <v>234</v>
       </c>
       <c r="C94" t="s">
-        <v>92</v>
+        <v>233</v>
       </c>
     </row>
     <row r="95" spans="1:291" s="5" customFormat="1">
       <c r="A95" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B95" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="C95" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D95" s="10"/>
       <c r="E95" s="10"/>
@@ -10004,520 +10755,522 @@
       <c r="KE95" s="10"/>
     </row>
     <row r="96" spans="1:291">
-      <c r="A96" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B96" s="5"/>
-      <c r="C96" s="5" t="s">
-        <v>245</v>
+      <c r="A96" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B96" t="s">
+        <v>238</v>
+      </c>
+      <c r="C96" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B97" t="s">
+        <v>240</v>
+      </c>
+      <c r="C97" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B98" t="s">
+        <v>241</v>
+      </c>
+      <c r="C98" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B99" t="s">
+        <v>91</v>
+      </c>
+      <c r="C99" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B100" t="s">
+        <v>244</v>
+      </c>
+      <c r="C100" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B101" s="5"/>
+      <c r="C101" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B102" t="s">
         <v>93</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C102" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
-      <c r="A98" s="4" t="s">
+    <row r="103" spans="1:3">
+      <c r="A103" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B98" s="5"/>
-      <c r="C98" s="5" t="s">
+      <c r="B103" s="5"/>
+      <c r="C103" s="5" t="s">
         <v>411</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" s="8" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B101" t="s">
-        <v>251</v>
-      </c>
-      <c r="C101" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B102" t="s">
-        <v>254</v>
-      </c>
-      <c r="C102" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B103" t="s">
-        <v>256</v>
-      </c>
-      <c r="C103" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104" s="8">
-        <v>1</v>
-      </c>
-      <c r="B104" t="s">
-        <v>259</v>
-      </c>
-      <c r="C104" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B105" t="s">
-        <v>5</v>
-      </c>
-      <c r="C105" t="s">
-        <v>277</v>
+        <v>246</v>
       </c>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="8">
+      <c r="A106" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B106" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C106" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B107" t="s">
+        <v>254</v>
+      </c>
+      <c r="C107" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B108" t="s">
+        <v>256</v>
+      </c>
+      <c r="C108" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="8">
+        <v>1</v>
+      </c>
+      <c r="B109" t="s">
+        <v>259</v>
+      </c>
+      <c r="C109" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B110" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="8">
+        <v>2</v>
+      </c>
+      <c r="B111" t="s">
+        <v>260</v>
+      </c>
+      <c r="C111" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B112" t="s">
         <v>6</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C112" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
-      <c r="A108" s="8">
+    <row r="113" spans="1:3">
+      <c r="A113" s="8">
         <v>3</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B113" t="s">
         <v>261</v>
       </c>
-      <c r="C108" s="14" t="s">
+      <c r="C113" s="14" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
-      <c r="A109" s="8" t="s">
+    <row r="114" spans="1:3">
+      <c r="A114" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B114" t="s">
         <v>7</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C114" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
-      <c r="A110" s="8">
+    <row r="115" spans="1:3">
+      <c r="A115" s="8">
         <v>4</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B115" t="s">
         <v>262</v>
       </c>
-      <c r="C110" s="14" t="s">
+      <c r="C115" s="14" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
-      <c r="A111" s="8" t="s">
+    <row r="116" spans="1:3">
+      <c r="A116" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B116" t="s">
         <v>8</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C116" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
-      <c r="A112" s="8">
+    <row r="117" spans="1:3">
+      <c r="A117" s="8">
         <v>5</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B117" t="s">
         <v>263</v>
       </c>
-      <c r="C112" s="14" t="s">
+      <c r="C117" s="14" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
-      <c r="A113" s="8" t="s">
+    <row r="118" spans="1:3">
+      <c r="A118" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B118" t="s">
         <v>9</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C118" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
-      <c r="A114" s="8">
+    <row r="119" spans="1:3">
+      <c r="A119" s="8">
         <v>6</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B119" t="s">
         <v>264</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C119" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
-      <c r="A115" s="8" t="s">
+    <row r="120" spans="1:3">
+      <c r="A120" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B120" t="s">
         <v>10</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C120" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
-      <c r="A116" s="8">
+    <row r="121" spans="1:3">
+      <c r="A121" s="8">
         <v>7</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B121" t="s">
         <v>265</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C121" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
-      <c r="A117" s="8" t="s">
+    <row r="122" spans="1:3">
+      <c r="A122" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B122" t="s">
         <v>11</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C122" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
-      <c r="A118" s="8">
+    <row r="123" spans="1:3">
+      <c r="A123" s="8">
         <v>8</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B123" t="s">
         <v>266</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C123" t="s">
         <v>275</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="A119" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B119" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="C119" s="15" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" s="8">
-        <v>9</v>
-      </c>
-      <c r="B120" t="s">
-        <v>267</v>
-      </c>
-      <c r="C120" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B121" s="17"/>
-      <c r="C121" s="17" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122" s="8">
-        <v>0</v>
-      </c>
-      <c r="B122" t="s">
-        <v>257</v>
-      </c>
-      <c r="C122" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B123" t="s">
-        <v>14</v>
-      </c>
-      <c r="C123" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B124" t="s">
-        <v>15</v>
-      </c>
-      <c r="C124" t="s">
-        <v>288</v>
+        <v>12</v>
+      </c>
+      <c r="B124" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="C124" s="15" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="8" t="s">
-        <v>16</v>
+      <c r="A125" s="8">
+        <v>9</v>
       </c>
       <c r="B125" t="s">
-        <v>16</v>
+        <v>267</v>
       </c>
       <c r="C125" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
     </row>
     <row r="126" spans="1:3">
-      <c r="A126" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B126" t="s">
-        <v>17</v>
-      </c>
-      <c r="C126" t="s">
-        <v>290</v>
+      <c r="A126" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B126" s="17"/>
+      <c r="C126" s="17" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="127" spans="1:3">
-      <c r="A127" s="8" t="s">
-        <v>18</v>
+      <c r="A127" s="8">
+        <v>0</v>
       </c>
       <c r="B127" t="s">
-        <v>19</v>
+        <v>257</v>
       </c>
       <c r="C127" t="s">
-        <v>291</v>
+        <v>258</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B128" t="s">
-        <v>293</v>
+        <v>14</v>
       </c>
       <c r="C128" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B129" t="s">
-        <v>294</v>
+        <v>15</v>
       </c>
       <c r="C129" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B130" t="s">
-        <v>297</v>
+        <v>16</v>
       </c>
       <c r="C130" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B131" t="s">
-        <v>299</v>
+        <v>17</v>
       </c>
       <c r="C131" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B132" t="s">
-        <v>301</v>
+        <v>19</v>
       </c>
       <c r="C132" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
     </row>
     <row r="133" spans="1:4" s="10" customFormat="1">
       <c r="A133" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B133" s="10" t="s">
-        <v>404</v>
-      </c>
-      <c r="C133" s="10" t="s">
-        <v>403</v>
+        <v>19</v>
+      </c>
+      <c r="B133" t="s">
+        <v>293</v>
+      </c>
+      <c r="C133" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B134" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="C134" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C135" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B136" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C136" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B137" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C137" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B138" t="s">
-        <v>310</v>
-      </c>
-      <c r="C138" t="s">
-        <v>311</v>
+        <v>24</v>
+      </c>
+      <c r="B138" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="C138" s="10" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B139" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C139" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B140" t="s">
-        <v>166</v>
+        <v>303</v>
       </c>
       <c r="C140" t="s">
-        <v>165</v>
+        <v>302</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B141" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="C141" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B142" t="s">
-        <v>97</v>
+        <v>307</v>
       </c>
       <c r="C142" t="s">
-        <v>98</v>
+        <v>306</v>
       </c>
     </row>
     <row r="143" spans="1:4">
-      <c r="A143" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>400</v>
+      <c r="A143" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B143" t="s">
+        <v>310</v>
+      </c>
+      <c r="C143" t="s">
+        <v>311</v>
       </c>
       <c r="D143" s="10" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="144" spans="1:4">
-      <c r="A144" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B144" s="5"/>
-      <c r="C144" s="5" t="s">
-        <v>316</v>
+      <c r="A144" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B144" t="s">
+        <v>313</v>
+      </c>
+      <c r="C144" t="s">
+        <v>312</v>
       </c>
       <c r="D144" s="10" t="s">
         <v>402</v>
@@ -10525,570 +11278,623 @@
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B145" t="s">
-        <v>318</v>
+        <v>166</v>
       </c>
       <c r="C145" t="s">
-        <v>317</v>
+        <v>165</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B146" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C146" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B147" t="s">
-        <v>322</v>
+        <v>97</v>
       </c>
       <c r="C147" t="s">
-        <v>321</v>
+        <v>98</v>
       </c>
     </row>
     <row r="148" spans="1:3">
-      <c r="A148" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B148" t="s">
-        <v>324</v>
-      </c>
-      <c r="C148" t="s">
-        <v>323</v>
+      <c r="A148" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="149" spans="1:3">
-      <c r="A149" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B149" t="s">
-        <v>40</v>
-      </c>
-      <c r="C149" t="s">
-        <v>325</v>
+      <c r="A149" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B149" s="5"/>
+      <c r="C149" s="5" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B150" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="C150" s="10" t="s">
-        <v>327</v>
+        <v>36</v>
+      </c>
+      <c r="B150" t="s">
+        <v>318</v>
+      </c>
+      <c r="C150" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B151" t="s">
-        <v>42</v>
+        <v>320</v>
       </c>
       <c r="C151" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B152" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="C152" s="10" t="s">
-        <v>328</v>
+        <v>38</v>
+      </c>
+      <c r="B152" t="s">
+        <v>322</v>
+      </c>
+      <c r="C152" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" s="8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B153" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C153" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B154" t="s">
-        <v>332</v>
+        <v>40</v>
       </c>
       <c r="C154" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B155" t="s">
-        <v>334</v>
-      </c>
-      <c r="C155" t="s">
-        <v>333</v>
+        <v>41</v>
+      </c>
+      <c r="B155" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="C155" s="10" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="156" spans="1:3" s="10" customFormat="1">
       <c r="A156" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B156" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="C156" s="10" t="s">
-        <v>399</v>
+        <v>42</v>
+      </c>
+      <c r="B156" t="s">
+        <v>42</v>
+      </c>
+      <c r="C156" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B157" t="s">
-        <v>336</v>
-      </c>
-      <c r="C157" t="s">
-        <v>335</v>
+        <v>43</v>
+      </c>
+      <c r="B157" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="C157" s="10" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B158" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C158" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B159" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="C159" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B160" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C160" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B161" t="s">
-        <v>346</v>
-      </c>
-      <c r="C161" t="s">
-        <v>345</v>
+        <v>47</v>
+      </c>
+      <c r="B161" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="C161" s="10" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B162" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="C162" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B163" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C163" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B164" s="10" t="s">
-        <v>397</v>
-      </c>
-      <c r="C164" s="10" t="s">
-        <v>396</v>
+        <v>50</v>
+      </c>
+      <c r="B164" t="s">
+        <v>342</v>
+      </c>
+      <c r="C164" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B165" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="C165" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B166" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C166" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B167" t="s">
-        <v>315</v>
+        <v>349</v>
       </c>
       <c r="C167" t="s">
-        <v>314</v>
+        <v>350</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B168" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="C168" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B169" s="10" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B170" s="10" t="s">
-        <v>393</v>
-      </c>
-      <c r="C170" s="10" t="s">
-        <v>392</v>
+        <v>56</v>
+      </c>
+      <c r="B170" t="s">
+        <v>347</v>
+      </c>
+      <c r="C170" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B171" t="s">
-        <v>184</v>
+        <v>352</v>
       </c>
       <c r="C171" t="s">
-        <v>183</v>
+        <v>351</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B172" t="s">
-        <v>63</v>
+        <v>315</v>
       </c>
       <c r="C172" t="s">
-        <v>355</v>
+        <v>314</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B173" t="s">
-        <v>64</v>
+        <v>354</v>
       </c>
       <c r="C173" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="174" spans="1:3">
-      <c r="A174" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B174" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C174" t="s">
-        <v>357</v>
+      <c r="A174" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B174" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="C174" s="10" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B175" t="s">
-        <v>359</v>
-      </c>
-      <c r="C175" t="s">
-        <v>358</v>
+        <v>61</v>
+      </c>
+      <c r="B175" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="C175" s="10" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B176" t="s">
-        <v>363</v>
+        <v>184</v>
       </c>
       <c r="C176" t="s">
-        <v>362</v>
+        <v>183</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B177" t="s">
-        <v>366</v>
+        <v>63</v>
       </c>
       <c r="C177" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B178" t="s">
-        <v>361</v>
+        <v>64</v>
       </c>
       <c r="C178" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="179" spans="1:3">
-      <c r="A179" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B179" t="s">
-        <v>369</v>
+      <c r="A179" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B179" s="18" t="s">
+        <v>65</v>
       </c>
       <c r="C179" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B180" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C180" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B181" s="19" t="s">
-        <v>391</v>
-      </c>
-      <c r="C181" s="10" t="s">
-        <v>370</v>
+        <v>66</v>
+      </c>
+      <c r="B181" t="s">
+        <v>363</v>
+      </c>
+      <c r="C181" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B182" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C182" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B183" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="C183" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B184" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C184" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B185" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="C185" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B186" t="s">
-        <v>379</v>
-      </c>
-      <c r="C186" t="s">
-        <v>380</v>
+        <v>72</v>
+      </c>
+      <c r="B186" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="C186" s="10" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B187" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="C187" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
     </row>
     <row r="188" spans="1:3" s="10" customFormat="1">
-      <c r="A188" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="C188" s="3" t="s">
-        <v>383</v>
+      <c r="A188" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B188" t="s">
+        <v>373</v>
+      </c>
+      <c r="C188" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B189" t="s">
-        <v>80</v>
+        <v>376</v>
       </c>
       <c r="C189" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
     </row>
     <row r="190" spans="1:3">
-      <c r="A190" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B190" s="13"/>
-      <c r="C190" s="13" t="s">
-        <v>405</v>
+      <c r="A190" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B190" t="s">
+        <v>378</v>
+      </c>
+      <c r="C190" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B191" t="s">
-        <v>84</v>
+        <v>379</v>
       </c>
       <c r="C191" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="192" spans="1:3">
-      <c r="A192" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B192" s="13"/>
-      <c r="C192" s="13" t="s">
-        <v>406</v>
+      <c r="A192" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B192" t="s">
+        <v>382</v>
+      </c>
+      <c r="C192" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="193" spans="1:3">
-      <c r="A193" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B193" t="s">
-        <v>84</v>
-      </c>
-      <c r="C193" t="s">
-        <v>388</v>
+      <c r="A193" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B194" t="s">
+        <v>80</v>
+      </c>
+      <c r="C194" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B195" s="13"/>
+      <c r="C195" s="13" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B196" t="s">
+        <v>84</v>
+      </c>
+      <c r="C196" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B197" s="13"/>
+      <c r="C197" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B198" t="s">
+        <v>84</v>
+      </c>
+      <c r="C198" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B199" t="s">
         <v>85</v>
       </c>
-      <c r="C194" t="s">
+      <c r="C199" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="195" spans="1:3">
-      <c r="A195" s="8"/>
-    </row>
-    <row r="196" spans="1:3">
-      <c r="A196" s="8"/>
-    </row>
-    <row r="197" spans="1:3">
-      <c r="A197" s="8"/>
-    </row>
-    <row r="198" spans="1:3">
-      <c r="A198" s="8"/>
-    </row>
-    <row r="199" spans="1:3">
-      <c r="A199" s="8"/>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" s="8"/>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" s="8"/>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" s="8"/>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" s="8"/>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" s="8"/>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" s="8"/>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Much of the main keyboard implemented.
</commit_message>
<xml_diff>
--- a/Resources/TranslationKeys.xlsx
+++ b/Resources/TranslationKeys.xlsx
@@ -1384,8 +1384,142 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="535">
+  <cellStyleXfs count="669">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1959,7 +2093,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="535">
+  <cellStyles count="669">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2227,6 +2361,73 @@
     <cellStyle name="Followed Hyperlink" xfId="530" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="532" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="534" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="536" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="538" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="540" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="546" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="548" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="550" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="552" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="578" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="580" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="596" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="604" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="608" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="610" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="612" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="614" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="620" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="624" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="626" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="628" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="630" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="632" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="634" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="636" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="638" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="664" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="668" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2494,6 +2695,73 @@
     <cellStyle name="Hyperlink" xfId="529" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="531" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="533" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="535" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="537" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="539" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="545" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="547" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="549" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="551" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="575" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="577" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="579" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="581" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="585" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="595" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="603" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="605" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="607" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="609" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="611" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="613" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="615" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="617" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="619" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="621" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="623" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="625" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="627" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="629" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="631" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="633" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="635" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="637" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="639" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="641" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="649" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="651" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="653" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="655" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="663" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="665" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="667" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2825,8 +3093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:KE206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Work towards confirming values.
</commit_message>
<xml_diff>
--- a/Resources/TranslationKeys.xlsx
+++ b/Resources/TranslationKeys.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="426">
   <si>
     <t>Arabic Name</t>
   </si>
@@ -789,9 +789,6 @@
     <t>DIVISION SIGN</t>
   </si>
   <si>
-    <t>0x00F7</t>
-  </si>
-  <si>
     <t>&amp;#x660</t>
   </si>
   <si>
@@ -876,9 +873,6 @@
     <t>ARABIC FIVE POINTED STAR</t>
   </si>
   <si>
-    <t xml:space="preserve">002A </t>
-  </si>
-  <si>
     <t>Dotted Line</t>
   </si>
   <si>
@@ -969,9 +963,6 @@
     <t>&amp;#xfdf1</t>
   </si>
   <si>
-    <t>High Yeh Baree</t>
-  </si>
-  <si>
     <t>Arabic Letter Teh Marbuta</t>
   </si>
   <si>
@@ -1194,9 +1185,6 @@
     <t>&amp;#FD3F</t>
   </si>
   <si>
-    <t>FDFC</t>
-  </si>
-  <si>
     <t>Arabic Small High Lam Alef</t>
   </si>
   <si>
@@ -1279,13 +1267,43 @@
   </si>
   <si>
     <t>&amp;#x62d</t>
+  </si>
+  <si>
+    <t>Arabic Small Yeh</t>
+  </si>
+  <si>
+    <t>&amp;#x6e6</t>
+  </si>
+  <si>
+    <t>Arabic Small High Yeh</t>
+  </si>
+  <si>
+    <t>&amp;#x6e7</t>
+  </si>
+  <si>
+    <t>Arabic Letter Heh Doachashmee Medial Form</t>
+  </si>
+  <si>
+    <t>&amp;#xfbad</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>&amp;x00F7</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>&amp;#1645;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1329,12 +1347,6 @@
       <sz val="12"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1384,8 +1396,292 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="669">
+  <cellStyleXfs count="953">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2084,16 +2380,18 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="669">
+  <cellStyles count="953">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2428,6 +2726,148 @@
     <cellStyle name="Followed Hyperlink" xfId="664" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="668" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="670" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="672" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="694" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="696" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="700" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="702" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="708" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="710" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="718" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="728" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="730" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="732" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="734" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="736" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="738" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="740" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="742" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="744" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="746" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="748" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="750" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="752" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="754" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="756" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="758" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="760" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="762" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="764" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="766" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="768" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="770" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="772" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="774" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="776" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="778" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="780" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="782" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="784" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="786" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="788" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="790" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="792" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="794" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="796" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="798" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="800" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="802" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="804" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="806" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="808" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="810" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="812" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="814" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="816" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="818" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="820" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="822" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="824" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="826" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="828" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="830" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="832" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="834" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="836" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="838" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="840" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="842" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="844" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="846" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="848" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="850" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="852" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="854" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="856" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="858" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="860" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="862" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="864" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="866" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="868" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="870" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="872" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="874" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="876" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="878" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="880" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="882" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="884" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="886" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="888" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="890" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="892" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="894" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="896" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="898" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="900" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="902" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="904" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="906" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="908" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="910" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="912" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="914" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="916" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="918" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="920" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="922" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="924" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="926" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="928" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="930" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="932" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="934" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="936" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="938" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="940" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="942" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="944" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="946" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="948" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="950" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="952" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2762,6 +3202,148 @@
     <cellStyle name="Hyperlink" xfId="663" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="665" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="667" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="669" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="671" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="675" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="707" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="709" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="711" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="717" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="725" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="727" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="729" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="731" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="733" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="735" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="737" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="739" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="741" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="743" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="745" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="747" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="749" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="751" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="753" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="755" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="757" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="759" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="761" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="763" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="765" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="767" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="769" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="771" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="773" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="775" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="777" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="779" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="781" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="783" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="785" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="787" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="789" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="791" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="793" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="795" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="797" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="799" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="801" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="803" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="805" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="807" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="809" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="811" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="813" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="815" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="817" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="819" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="821" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="823" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="825" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="827" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="829" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="831" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="833" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="835" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="837" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="839" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="841" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="843" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="845" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="847" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="849" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="851" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="853" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="855" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="857" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="859" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="861" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="863" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="865" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="867" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="869" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="871" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="873" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="875" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="877" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="879" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="881" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="883" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="885" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="887" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="889" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="891" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="893" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="895" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="897" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="899" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="901" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="903" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="905" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="907" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="909" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="911" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="913" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="915" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="917" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="919" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="921" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="923" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="925" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="927" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="929" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="931" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="933" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="935" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="937" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="939" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="941" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="943" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="945" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="947" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="949" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="951" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3093,8 +3675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:KE206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3118,6 +3700,9 @@
       <c r="C1" s="11" t="s">
         <v>250</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="2" spans="1:291">
       <c r="C2" s="10"/>
@@ -3138,25 +3723,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:291">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:291" s="10" customFormat="1">
+      <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:291" s="3" customFormat="1">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>88</v>
       </c>
       <c r="D6" s="10"/>
@@ -3449,13 +4034,13 @@
       <c r="KE6" s="10"/>
     </row>
     <row r="7" spans="1:291" s="3" customFormat="1">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="6" t="s">
         <v>90</v>
       </c>
       <c r="D7" s="10"/>
@@ -3748,24 +4333,24 @@
       <c r="KE7" s="10"/>
     </row>
     <row r="8" spans="1:291">
-      <c r="A8" s="1">
+      <c r="A8" s="15">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:291" s="3" customFormat="1">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="6" t="s">
         <v>128</v>
       </c>
       <c r="D9" s="10"/>
@@ -4058,24 +4643,24 @@
       <c r="KE9" s="10"/>
     </row>
     <row r="10" spans="1:291" s="10" customFormat="1">
-      <c r="A10" s="8">
+      <c r="A10" s="15">
         <v>2</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="6" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:291" s="3" customFormat="1">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>130</v>
       </c>
       <c r="D11" s="10"/>
@@ -4368,24 +4953,24 @@
       <c r="KE11" s="10"/>
     </row>
     <row r="12" spans="1:291" s="10" customFormat="1">
-      <c r="A12" s="8">
+      <c r="A12" s="15">
         <v>3</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="6" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:291" s="3" customFormat="1">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B13" t="s">
-        <v>418</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>170</v>
       </c>
       <c r="D13" s="10"/>
@@ -4689,14 +5274,14 @@
       </c>
     </row>
     <row r="15" spans="1:291" s="3" customFormat="1">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>412</v>
+      <c r="B15" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>408</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -4988,24 +5573,24 @@
       <c r="KE15" s="10"/>
     </row>
     <row r="16" spans="1:291" s="10" customFormat="1">
-      <c r="A16" s="8">
+      <c r="A16" s="15">
         <v>5</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:291" s="3" customFormat="1">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="6" t="s">
         <v>106</v>
       </c>
       <c r="D17" s="10"/>
@@ -5309,13 +5894,13 @@
       </c>
     </row>
     <row r="19" spans="1:291" s="3" customFormat="1">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="6" t="s">
         <v>132</v>
       </c>
       <c r="D19" s="10"/>
@@ -5619,13 +6204,13 @@
       </c>
     </row>
     <row r="21" spans="1:291" s="3" customFormat="1">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="6" t="s">
         <v>136</v>
       </c>
       <c r="D21" s="10"/>
@@ -5918,24 +6503,24 @@
       <c r="KE21" s="10"/>
     </row>
     <row r="22" spans="1:291" s="10" customFormat="1">
-      <c r="A22" s="8">
+      <c r="A22" s="15">
         <v>8</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="6" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:291" s="3" customFormat="1">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D23" s="10"/>
@@ -6228,79 +6813,79 @@
       <c r="KE23" s="10"/>
     </row>
     <row r="24" spans="1:291" s="10" customFormat="1">
-      <c r="A24" s="8">
+      <c r="A24" s="15">
         <v>9</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="6" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:291">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="6" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:291" s="10" customFormat="1">
-      <c r="A26" s="8">
+      <c r="A26" s="15">
         <v>0</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="6" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:291">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="19" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:291">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="19" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:291">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B29" t="s">
-        <v>416</v>
-      </c>
-      <c r="C29" t="s">
-        <v>415</v>
+      <c r="B29" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="30" spans="1:291" s="5" customFormat="1">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="6" t="s">
         <v>141</v>
       </c>
       <c r="D30" s="10"/>
@@ -6593,24 +7178,24 @@
       <c r="KE30" s="10"/>
     </row>
     <row r="31" spans="1:291">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="3" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:291">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="6" t="s">
         <v>145</v>
       </c>
     </row>
@@ -7295,7 +7880,7 @@
         <v>162</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="44" spans="1:291" s="3" customFormat="1">
@@ -8332,7 +8917,7 @@
         <v>19</v>
       </c>
       <c r="B59" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C59" t="s">
         <v>145</v>
@@ -8990,10 +9575,10 @@
         <v>50</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="68" spans="1:291">
@@ -9322,7 +9907,7 @@
         <v>54</v>
       </c>
       <c r="B71" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C71" t="s">
         <v>102</v>
@@ -9621,10 +10206,10 @@
         <v>55</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>397</v>
+        <v>421</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>396</v>
+        <v>420</v>
       </c>
     </row>
     <row r="73" spans="1:291">
@@ -9973,10 +10558,10 @@
         <v>61</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="79" spans="1:291">
@@ -11103,7 +11688,7 @@
       </c>
       <c r="B103" s="5"/>
       <c r="C103" s="5" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -11112,287 +11697,289 @@
       </c>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="8" t="s">
+      <c r="A106" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="6" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="8" t="s">
+      <c r="A107" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="6" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="8" t="s">
+      <c r="A108" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="15">
+        <v>1</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="15">
+        <v>2</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="15">
+        <v>3</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="C113" s="16" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="15">
+        <v>4</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C115" s="16" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="15">
+        <v>5</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="C117" s="16" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="15">
+        <v>6</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="15">
+        <v>7</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="15">
+        <v>8</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B124" s="17" t="s">
+        <v>425</v>
+      </c>
+      <c r="C124" s="17" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="15">
+        <v>9</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B126" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="C126" s="19" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="15">
+        <v>0</v>
+      </c>
+      <c r="B127" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="C108" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" s="8">
-        <v>1</v>
-      </c>
-      <c r="B109" t="s">
-        <v>259</v>
-      </c>
-      <c r="C109" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B110" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="A111" s="8">
-        <v>2</v>
-      </c>
-      <c r="B111" t="s">
-        <v>260</v>
-      </c>
-      <c r="C111" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="A112" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B112" t="s">
-        <v>6</v>
-      </c>
-      <c r="C112" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113" s="8">
-        <v>3</v>
-      </c>
-      <c r="B113" t="s">
-        <v>261</v>
-      </c>
-      <c r="C113" s="14" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="A114" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B114" t="s">
-        <v>7</v>
-      </c>
-      <c r="C114" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115" s="8">
-        <v>4</v>
-      </c>
-      <c r="B115" t="s">
-        <v>262</v>
-      </c>
-      <c r="C115" s="14" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B116" t="s">
-        <v>8</v>
-      </c>
-      <c r="C116" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" s="8">
-        <v>5</v>
-      </c>
-      <c r="B117" t="s">
-        <v>263</v>
-      </c>
-      <c r="C117" s="14" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="A118" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B118" t="s">
-        <v>9</v>
-      </c>
-      <c r="C118" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="A119" s="8">
-        <v>6</v>
-      </c>
-      <c r="B119" t="s">
-        <v>264</v>
-      </c>
-      <c r="C119" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B120" t="s">
-        <v>10</v>
-      </c>
-      <c r="C120" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" s="8">
-        <v>7</v>
-      </c>
-      <c r="B121" t="s">
-        <v>265</v>
-      </c>
-      <c r="C121" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B122" t="s">
-        <v>11</v>
-      </c>
-      <c r="C122" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123" s="8">
-        <v>8</v>
-      </c>
-      <c r="B123" t="s">
-        <v>266</v>
-      </c>
-      <c r="C123" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="A124" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B124" s="15" t="s">
+      <c r="C127" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C128" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C124" s="15" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3">
-      <c r="A125" s="8">
-        <v>9</v>
-      </c>
-      <c r="B125" t="s">
-        <v>267</v>
-      </c>
-      <c r="C125" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3">
-      <c r="A126" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B126" s="17"/>
-      <c r="C126" s="17" t="s">
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C129" s="3" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
-      <c r="A127" s="8">
-        <v>0</v>
-      </c>
-      <c r="B127" t="s">
-        <v>257</v>
-      </c>
-      <c r="C127" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
-      <c r="A128" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B128" t="s">
-        <v>14</v>
-      </c>
-      <c r="C128" t="s">
+    <row r="130" spans="1:4">
+      <c r="A130" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C130" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
-      <c r="A129" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B129" t="s">
-        <v>15</v>
-      </c>
-      <c r="C129" t="s">
+    <row r="131" spans="1:4">
+      <c r="A131" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C131" s="6" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4">
-      <c r="A130" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B130" t="s">
-        <v>16</v>
-      </c>
-      <c r="C130" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4">
-      <c r="A131" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B131" t="s">
-        <v>17</v>
-      </c>
-      <c r="C131" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -11403,7 +11990,7 @@
         <v>19</v>
       </c>
       <c r="C132" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="133" spans="1:4" s="10" customFormat="1">
@@ -11411,10 +11998,10 @@
         <v>19</v>
       </c>
       <c r="B133" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C133" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -11422,10 +12009,10 @@
         <v>20</v>
       </c>
       <c r="B134" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C134" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -11433,10 +12020,10 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C135" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -11444,10 +12031,10 @@
         <v>22</v>
       </c>
       <c r="B136" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C136" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -11455,10 +12042,10 @@
         <v>23</v>
       </c>
       <c r="B137" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C137" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -11466,10 +12053,10 @@
         <v>24</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C138" s="10" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -11477,10 +12064,10 @@
         <v>25</v>
       </c>
       <c r="B139" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C139" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -11488,10 +12075,10 @@
         <v>26</v>
       </c>
       <c r="B140" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C140" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -11499,10 +12086,10 @@
         <v>27</v>
       </c>
       <c r="B141" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C141" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -11510,10 +12097,10 @@
         <v>28</v>
       </c>
       <c r="B142" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C142" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -11521,13 +12108,13 @@
         <v>29</v>
       </c>
       <c r="B143" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C143" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D143" s="10" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -11535,13 +12122,13 @@
         <v>30</v>
       </c>
       <c r="B144" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C144" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D144" s="10" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -11549,10 +12136,10 @@
         <v>31</v>
       </c>
       <c r="B145" t="s">
-        <v>166</v>
+        <v>417</v>
       </c>
       <c r="C145" t="s">
-        <v>165</v>
+        <v>416</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -11560,10 +12147,10 @@
         <v>32</v>
       </c>
       <c r="B146" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C146" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -11582,19 +12169,21 @@
         <v>34</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B149" s="5"/>
+      <c r="B149" s="5" t="s">
+        <v>419</v>
+      </c>
       <c r="C149" s="5" t="s">
-        <v>316</v>
+        <v>418</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -11602,10 +12191,10 @@
         <v>36</v>
       </c>
       <c r="B150" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C150" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -11613,10 +12202,10 @@
         <v>37</v>
       </c>
       <c r="B151" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C151" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -11624,10 +12213,10 @@
         <v>38</v>
       </c>
       <c r="B152" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C152" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -11635,10 +12224,10 @@
         <v>39</v>
       </c>
       <c r="B153" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C153" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -11649,7 +12238,7 @@
         <v>40</v>
       </c>
       <c r="C154" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -11657,10 +12246,10 @@
         <v>41</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C155" s="10" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="156" spans="1:3" s="10" customFormat="1">
@@ -11671,7 +12260,7 @@
         <v>42</v>
       </c>
       <c r="C156" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -11679,10 +12268,10 @@
         <v>43</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C157" s="10" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -11690,10 +12279,10 @@
         <v>44</v>
       </c>
       <c r="B158" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C158" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -11701,10 +12290,10 @@
         <v>45</v>
       </c>
       <c r="B159" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C159" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -11712,10 +12301,10 @@
         <v>46</v>
       </c>
       <c r="B160" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C160" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -11723,10 +12312,10 @@
         <v>47</v>
       </c>
       <c r="B161" s="10" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C161" s="10" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -11734,10 +12323,10 @@
         <v>48</v>
       </c>
       <c r="B162" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C162" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -11745,10 +12334,10 @@
         <v>49</v>
       </c>
       <c r="B163" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C163" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -11756,10 +12345,10 @@
         <v>50</v>
       </c>
       <c r="B164" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C164" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -11767,10 +12356,10 @@
         <v>51</v>
       </c>
       <c r="B165" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C165" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -11778,10 +12367,10 @@
         <v>52</v>
       </c>
       <c r="B166" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C166" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -11789,10 +12378,10 @@
         <v>53</v>
       </c>
       <c r="B167" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C167" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -11800,10 +12389,10 @@
         <v>54</v>
       </c>
       <c r="B168" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C168" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -11811,10 +12400,10 @@
         <v>55</v>
       </c>
       <c r="B169" s="10" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -11822,10 +12411,10 @@
         <v>56</v>
       </c>
       <c r="B170" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C170" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -11833,10 +12422,10 @@
         <v>57</v>
       </c>
       <c r="B171" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C171" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -11844,10 +12433,10 @@
         <v>58</v>
       </c>
       <c r="B172" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C172" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -11855,10 +12444,10 @@
         <v>59</v>
       </c>
       <c r="B173" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C173" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -11866,10 +12455,10 @@
         <v>60</v>
       </c>
       <c r="B174" s="10" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C174" s="10" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -11877,10 +12466,10 @@
         <v>61</v>
       </c>
       <c r="B175" s="10" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C175" s="10" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -11902,7 +12491,7 @@
         <v>63</v>
       </c>
       <c r="C177" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -11913,18 +12502,18 @@
         <v>64</v>
       </c>
       <c r="C178" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B179" s="18" t="s">
+      <c r="B179" s="14" t="s">
         <v>65</v>
       </c>
       <c r="C179" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -11932,10 +12521,10 @@
         <v>67</v>
       </c>
       <c r="B180" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C180" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -11943,10 +12532,10 @@
         <v>66</v>
       </c>
       <c r="B181" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C181" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -11954,10 +12543,10 @@
         <v>68</v>
       </c>
       <c r="B182" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C182" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -11965,10 +12554,10 @@
         <v>69</v>
       </c>
       <c r="B183" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C183" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -11976,10 +12565,10 @@
         <v>70</v>
       </c>
       <c r="B184" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C184" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -11987,21 +12576,21 @@
         <v>71</v>
       </c>
       <c r="B185" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C185" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B186" s="19" t="s">
-        <v>391</v>
+      <c r="B186" t="s">
+        <v>366</v>
       </c>
       <c r="C186" s="10" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -12009,10 +12598,10 @@
         <v>73</v>
       </c>
       <c r="B187" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C187" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="188" spans="1:3" s="10" customFormat="1">
@@ -12020,10 +12609,10 @@
         <v>74</v>
       </c>
       <c r="B188" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C188" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -12031,10 +12620,10 @@
         <v>75</v>
       </c>
       <c r="B189" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C189" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -12042,10 +12631,10 @@
         <v>76</v>
       </c>
       <c r="B190" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C190" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -12053,10 +12642,10 @@
         <v>77</v>
       </c>
       <c r="B191" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C191" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -12064,10 +12653,10 @@
         <v>78</v>
       </c>
       <c r="B192" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C192" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -12075,10 +12664,10 @@
         <v>79</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -12089,7 +12678,7 @@
         <v>80</v>
       </c>
       <c r="C194" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -12098,7 +12687,7 @@
       </c>
       <c r="B195" s="13"/>
       <c r="C195" s="13" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -12106,10 +12695,10 @@
         <v>82</v>
       </c>
       <c r="B196" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C196" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -12118,7 +12707,7 @@
       </c>
       <c r="B197" s="13"/>
       <c r="C197" s="13" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -12129,7 +12718,7 @@
         <v>84</v>
       </c>
       <c r="C198" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -12140,7 +12729,7 @@
         <v>85</v>
       </c>
       <c r="C199" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="200" spans="1:3">

</xml_diff>

<commit_message>
More values found and everything else confirmed.
</commit_message>
<xml_diff>
--- a/Resources/TranslationKeys.xlsx
+++ b/Resources/TranslationKeys.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="445">
   <si>
     <t>Arabic Name</t>
   </si>
@@ -318,12 +318,6 @@
     <t>Arabic Letter Yeh With Hamza Above</t>
   </si>
   <si>
-    <t>Arabic Thousands Separator</t>
-  </si>
-  <si>
-    <t>&amp;#x66c</t>
-  </si>
-  <si>
     <t>&amp;#x6af</t>
   </si>
   <si>
@@ -552,12 +546,6 @@
     <t>&amp;#x6c1</t>
   </si>
   <si>
-    <t>Arabic Small Damma</t>
-  </si>
-  <si>
-    <t>&amp;#x619</t>
-  </si>
-  <si>
     <t>Arabic Letter Peh</t>
   </si>
   <si>
@@ -645,9 +633,6 @@
     <t>Arabic Semicolon</t>
   </si>
   <si>
-    <t>&amp;#x640</t>
-  </si>
-  <si>
     <t>Arabic Tatweel</t>
   </si>
   <si>
@@ -741,18 +726,9 @@
     <t>&amp;#x645</t>
   </si>
   <si>
-    <t>&amp;#x61a</t>
-  </si>
-  <si>
-    <t>Arabic Small Kasra</t>
-  </si>
-  <si>
     <t>Arabic Small Fatha</t>
   </si>
   <si>
-    <t>&amp;#x618</t>
-  </si>
-  <si>
     <t>Urdu Full Stop</t>
   </si>
   <si>
@@ -873,12 +849,6 @@
     <t>Dotted Line</t>
   </si>
   <si>
-    <t>"low minus"</t>
-  </si>
-  <si>
-    <t>"hyphen minus"</t>
-  </si>
-  <si>
     <t>Plus sign</t>
   </si>
   <si>
@@ -933,9 +903,6 @@
     <t>TRADE MARK SIGN</t>
   </si>
   <si>
-    <t>&amp;#2122</t>
-  </si>
-  <si>
     <t>&amp;#x60f</t>
   </si>
   <si>
@@ -1224,9 +1191,6 @@
     <t>Number Comma</t>
   </si>
   <si>
-    <t>English Full Stop</t>
-  </si>
-  <si>
     <t>Arabic Subscript Alef</t>
   </si>
   <si>
@@ -1297,6 +1261,99 @@
   </si>
   <si>
     <t>right square bracket</t>
+  </si>
+  <si>
+    <t>looks slightly different</t>
+  </si>
+  <si>
+    <t>isn't sideways</t>
+  </si>
+  <si>
+    <t>isn't above the center</t>
+  </si>
+  <si>
+    <t>can't find</t>
+  </si>
+  <si>
+    <t>no dot.</t>
+  </si>
+  <si>
+    <t>&amp;#x64f</t>
+  </si>
+  <si>
+    <t>Arabic Damma</t>
+  </si>
+  <si>
+    <t>left single quote</t>
+  </si>
+  <si>
+    <t>right single quote</t>
+  </si>
+  <si>
+    <t>&amp;#x2018</t>
+  </si>
+  <si>
+    <t>&amp;#x2019</t>
+  </si>
+  <si>
+    <t>&amp;#x653;</t>
+  </si>
+  <si>
+    <t>not appearing on the top</t>
+  </si>
+  <si>
+    <t>Found, but not working well (not included in the keybaord)</t>
+  </si>
+  <si>
+    <t>not appearing propperly</t>
+  </si>
+  <si>
+    <t>lig</t>
+  </si>
+  <si>
+    <t>&amp;#x640;</t>
+  </si>
+  <si>
+    <t>These two look the same</t>
+  </si>
+  <si>
+    <t>&amp;#xfe7a</t>
+  </si>
+  <si>
+    <t>Arabic Kasra Isolated Form</t>
+  </si>
+  <si>
+    <t>&amp;#x64e</t>
+  </si>
+  <si>
+    <t>&amp;#x2212;</t>
+  </si>
+  <si>
+    <t>minus sign</t>
+  </si>
+  <si>
+    <t>hyphen minus</t>
+  </si>
+  <si>
+    <t>not sure what "low minus" is</t>
+  </si>
+  <si>
+    <t>&amp;#x2122;</t>
+  </si>
+  <si>
+    <t>not showing up</t>
+  </si>
+  <si>
+    <t>has an extra line after (I think</t>
+  </si>
+  <si>
+    <t>full stop</t>
+  </si>
+  <si>
+    <t>&amp;#x2e</t>
+  </si>
+  <si>
+    <t>doesn't show up for some reason</t>
   </si>
 </sst>
 </file>
@@ -1382,7 +1439,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1396,7 +1453,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="953">
+  <cellStyleXfs count="999">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2350,8 +2407,54 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2376,11 +2479,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2390,8 +2488,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="953">
+  <cellStyles count="999">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2868,6 +2974,29 @@
     <cellStyle name="Followed Hyperlink" xfId="948" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="950" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="952" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="954" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="956" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="958" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="960" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="962" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="964" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="966" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="968" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="970" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="972" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="974" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="976" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="978" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="980" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="982" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="984" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="986" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="988" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="990" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="992" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="994" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="996" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="998" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3344,6 +3473,29 @@
     <cellStyle name="Hyperlink" xfId="947" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="949" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="951" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="953" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="955" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="957" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="959" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="961" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="963" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="965" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="967" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="969" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="971" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="973" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="975" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="977" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="979" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="981" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="983" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="985" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="987" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="989" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="991" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="993" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="995" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="997" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3675,8 +3827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:KE206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="C197" sqref="C197"/>
+    <sheetView tabSelected="1" topLeftCell="B182" workbookViewId="0">
+      <selection activeCell="D204" sqref="D204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3684,7 +3836,7 @@
     <col min="1" max="1" width="19.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="52.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="29" style="10" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="10"/>
     <col min="6" max="6" width="12" style="10" customWidth="1"/>
     <col min="7" max="291" width="10.83203125" style="10"/>
@@ -3692,24 +3844,26 @@
   <sheetData>
     <row r="1" spans="1:291">
       <c r="A1" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>423</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:291">
-      <c r="C2" s="10"/>
+      <c r="A2" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="3" spans="1:291">
       <c r="A3" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:291" s="10" customFormat="1">
@@ -3717,14 +3871,14 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:291" s="10" customFormat="1">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -3735,7 +3889,7 @@
       </c>
     </row>
     <row r="6" spans="1:291" s="3" customFormat="1">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -4034,7 +4188,7 @@
       <c r="KE6" s="10"/>
     </row>
     <row r="7" spans="1:291" s="3" customFormat="1">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -4333,25 +4487,25 @@
       <c r="KE7" s="10"/>
     </row>
     <row r="8" spans="1:291">
-      <c r="A8" s="15">
+      <c r="A8" s="12">
         <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:291" s="3" customFormat="1">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>81</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -4643,25 +4797,25 @@
       <c r="KE9" s="10"/>
     </row>
     <row r="10" spans="1:291" s="10" customFormat="1">
-      <c r="A10" s="15">
+      <c r="A10" s="12">
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:291" s="3" customFormat="1">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -4953,25 +5107,25 @@
       <c r="KE11" s="10"/>
     </row>
     <row r="12" spans="1:291" s="10" customFormat="1">
-      <c r="A12" s="15">
+      <c r="A12" s="12">
         <v>3</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:291" s="3" customFormat="1">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -5267,21 +5421,24 @@
         <v>4</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="15" spans="1:291" s="3" customFormat="1">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -5573,25 +5730,25 @@
       <c r="KE15" s="10"/>
     </row>
     <row r="16" spans="1:291" s="10" customFormat="1">
-      <c r="A16" s="15">
+      <c r="A16" s="12">
         <v>5</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:291" s="3" customFormat="1">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -5883,25 +6040,25 @@
       <c r="KE17" s="10"/>
     </row>
     <row r="18" spans="1:291">
-      <c r="A18" s="2">
+      <c r="A18" s="12">
         <v>6</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>117</v>
+      <c r="B18" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:291" s="3" customFormat="1">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -6197,21 +6354,24 @@
         <v>7</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="21" spans="1:291" s="3" customFormat="1">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -6503,25 +6663,25 @@
       <c r="KE21" s="10"/>
     </row>
     <row r="22" spans="1:291" s="10" customFormat="1">
-      <c r="A22" s="15">
+      <c r="A22" s="12">
         <v>8</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:291" s="3" customFormat="1">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -6813,80 +6973,80 @@
       <c r="KE23" s="10"/>
     </row>
     <row r="24" spans="1:291" s="10" customFormat="1">
-      <c r="A24" s="15">
+      <c r="A24" s="12">
         <v>9</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:291">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:291" s="10" customFormat="1">
-      <c r="A26" s="15">
+      <c r="A26" s="12">
         <v>0</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:291">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:291">
+      <c r="A28" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="C27" s="19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="28" spans="1:291">
-      <c r="A28" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="19" t="s">
+    </row>
+    <row r="29" spans="1:291">
+      <c r="A29" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:291" s="5" customFormat="1">
+      <c r="A30" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>139</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="29" spans="1:291">
-      <c r="A29" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>411</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="30" spans="1:291" s="5" customFormat="1">
-      <c r="A30" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
@@ -7182,21 +7342,24 @@
         <v>18</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="32" spans="1:291">
+      <c r="A32" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C32" s="6" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="32" spans="1:291">
-      <c r="A32" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:291" s="5" customFormat="1">
@@ -7204,9 +7367,11 @@
         <v>20</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="D34" s="10"/>
+        <v>145</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>417</v>
+      </c>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
@@ -7496,36 +7661,36 @@
       <c r="KE34" s="10"/>
     </row>
     <row r="35" spans="1:291">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:291">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:291">
+      <c r="A37" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C37" s="6" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="37" spans="1:291">
-      <c r="A37" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:291">
@@ -7534,29 +7699,29 @@
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:291">
+      <c r="A39" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="39" spans="1:291">
-      <c r="A39" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="6" t="s">
+      <c r="C39" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:291" s="3" customFormat="1">
+      <c r="A40" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>154</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="40" spans="1:291" s="3" customFormat="1">
-      <c r="A40" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>156</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
@@ -7848,39 +8013,39 @@
       <c r="KE40" s="10"/>
     </row>
     <row r="41" spans="1:291">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="1:291">
+      <c r="A42" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="1:291">
-      <c r="A42" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B42" s="6" t="s">
+    </row>
+    <row r="43" spans="1:291">
+      <c r="A43" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="43" spans="1:291">
-      <c r="A43" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>162</v>
-      </c>
       <c r="D43" s="10" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
     </row>
     <row r="44" spans="1:291" s="3" customFormat="1">
@@ -7888,12 +8053,14 @@
         <v>30</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D44" s="10"/>
+        <v>161</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>418</v>
+      </c>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
@@ -8183,69 +8350,69 @@
       <c r="KE44" s="10"/>
     </row>
     <row r="45" spans="1:291">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B45" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="46" spans="1:291">
+      <c r="A46" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C46" s="6" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:291">
-      <c r="A46" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B46" s="6" t="s">
+    <row r="47" spans="1:291">
+      <c r="A47" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="47" spans="1:291">
-      <c r="A47" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B47" s="6" t="s">
+    </row>
+    <row r="48" spans="1:291">
+      <c r="A48" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="48" spans="1:291">
-      <c r="A48" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="6" t="s">
+    </row>
+    <row r="49" spans="1:291">
+      <c r="A49" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:291" s="6" customFormat="1">
+      <c r="A50" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C50" s="6" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="49" spans="1:291">
-      <c r="A49" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="50" spans="1:291" s="6" customFormat="1">
-      <c r="A50" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>173</v>
       </c>
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
@@ -8537,25 +8704,25 @@
       <c r="KE50" s="10"/>
     </row>
     <row r="51" spans="1:291">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="1:291" s="6" customFormat="1">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B52" t="s">
-        <v>178</v>
-      </c>
-      <c r="C52" t="s">
-        <v>177</v>
+      <c r="B52" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>420</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
@@ -8847,80 +9014,80 @@
       <c r="KE52" s="10"/>
     </row>
     <row r="53" spans="1:291">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="54" spans="1:291">
       <c r="A54" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B54" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>99</v>
+      <c r="B54" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="55" spans="1:291">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="12" t="s">
         <v>41</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="56" spans="1:291">
       <c r="A56" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B56" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="C56" s="13" t="s">
-        <v>92</v>
+      <c r="B56" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="57" spans="1:291">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="12" t="s">
         <v>43</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
     </row>
     <row r="58" spans="1:291">
-      <c r="A58" s="15" t="s">
+      <c r="A58" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C58" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:291">
+      <c r="A59" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="C59" s="6" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="59" spans="1:291">
-      <c r="A59" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>412</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:291" s="5" customFormat="1">
@@ -9221,14 +9388,17 @@
         <v>44</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>183</v>
+        <v>425</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="62" spans="1:291">
-      <c r="A62" s="15" t="s">
+      <c r="A62" s="12" t="s">
         <v>45</v>
       </c>
       <c r="B62" s="6" t="s">
@@ -9239,36 +9409,39 @@
       </c>
     </row>
     <row r="63" spans="1:291">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="64" spans="1:291">
+      <c r="A64" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="65" spans="1:291" s="5" customFormat="1">
+      <c r="A65" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C65" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="C63" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="64" spans="1:291">
-      <c r="A64" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="65" spans="1:291" s="5" customFormat="1">
-      <c r="A65" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="D65" s="10"/>
       <c r="E65" s="10"/>
@@ -9560,58 +9733,58 @@
       <c r="KE65" s="10"/>
     </row>
     <row r="66" spans="1:291">
-      <c r="A66" s="15" t="s">
+      <c r="A66" s="12" t="s">
         <v>49</v>
       </c>
       <c r="B66" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="67" spans="1:291">
+      <c r="A67" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="68" spans="1:291">
+      <c r="A68" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="69" spans="1:291">
+      <c r="A69" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B69" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C69" s="6" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="67" spans="1:291">
-      <c r="A67" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="68" spans="1:291">
-      <c r="A68" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="69" spans="1:291">
-      <c r="A69" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
     <row r="70" spans="1:291" s="5" customFormat="1">
-      <c r="A70" s="15" t="s">
+      <c r="A70" s="12" t="s">
         <v>53</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D70" s="10"/>
       <c r="E70" s="10"/>
@@ -9903,14 +10076,14 @@
       <c r="KE70" s="10"/>
     </row>
     <row r="71" spans="1:291" s="5" customFormat="1">
-      <c r="A71" s="15" t="s">
+      <c r="A71" s="12" t="s">
         <v>54</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71" s="10"/>
@@ -10202,47 +10375,47 @@
       <c r="KE71" s="10"/>
     </row>
     <row r="72" spans="1:291">
-      <c r="A72" s="15" t="s">
+      <c r="A72" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
     </row>
     <row r="73" spans="1:291">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="74" spans="1:291">
+      <c r="A74" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="75" spans="1:291" s="3" customFormat="1">
+      <c r="A75" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B75" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C75" s="6" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="74" spans="1:291">
-      <c r="A74" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="75" spans="1:291" s="3" customFormat="1">
-      <c r="A75" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>200</v>
       </c>
       <c r="D75" s="10"/>
       <c r="E75" s="10"/>
@@ -10534,14 +10707,14 @@
       <c r="KE75" s="10"/>
     </row>
     <row r="76" spans="1:291">
-      <c r="A76" s="15" t="s">
+      <c r="A76" s="12" t="s">
         <v>59</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="77" spans="1:291">
@@ -10550,51 +10723,57 @@
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5" t="s">
-        <v>204</v>
+        <v>200</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="78" spans="1:291">
-      <c r="A78" s="15" t="s">
+      <c r="A78" s="12" t="s">
         <v>61</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
     </row>
     <row r="79" spans="1:291">
-      <c r="A79" s="15" t="s">
+      <c r="A79" s="12" t="s">
         <v>62</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="80" spans="1:291">
-      <c r="A80" s="15" t="s">
+      <c r="A80" s="12" t="s">
         <v>63</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="81" spans="1:291">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B81" t="s">
-        <v>208</v>
-      </c>
-      <c r="C81" t="s">
-        <v>209</v>
+      <c r="B81" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="82" spans="1:291">
@@ -10602,26 +10781,29 @@
         <v>65</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>211</v>
+        <v>206</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="83" spans="1:291">
-      <c r="A83" s="7"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
+      <c r="A83" s="9"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
     </row>
     <row r="84" spans="1:291" s="5" customFormat="1">
-      <c r="A84" s="15" t="s">
+      <c r="A84" s="12" t="s">
         <v>67</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D84" s="10"/>
       <c r="E84" s="10"/>
@@ -10913,80 +11095,80 @@
       <c r="KE84" s="10"/>
     </row>
     <row r="85" spans="1:291">
-      <c r="A85" s="15" t="s">
+      <c r="A85" s="12" t="s">
         <v>66</v>
       </c>
       <c r="B85" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="86" spans="1:291">
+      <c r="A86" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="87" spans="1:291">
+      <c r="A87" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="88" spans="1:291">
+      <c r="A88" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B88" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C85" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="86" spans="1:291">
-      <c r="A86" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B86" s="6" t="s">
+      <c r="C88" s="6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="89" spans="1:291">
+      <c r="A89" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C89" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C86" s="6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="87" spans="1:291">
-      <c r="A87" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C87" s="6" t="s">
+    </row>
+    <row r="90" spans="1:291">
+      <c r="A90" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C90" s="6" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="88" spans="1:291">
-      <c r="A88" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="C88" s="6" t="s">
+    <row r="91" spans="1:291">
+      <c r="A91" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C91" s="6" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="89" spans="1:291">
-      <c r="A89" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="90" spans="1:291">
-      <c r="A90" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="91" spans="1:291">
-      <c r="A91" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="92" spans="1:291">
@@ -10995,18 +11177,21 @@
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="93" spans="1:291" s="5" customFormat="1">
-      <c r="A93" s="15" t="s">
+      <c r="A93" s="12" t="s">
         <v>75</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D93" s="10"/>
       <c r="E93" s="10"/>
@@ -11298,25 +11483,25 @@
       <c r="KE93" s="10"/>
     </row>
     <row r="94" spans="1:291">
-      <c r="A94" s="15" t="s">
+      <c r="A94" s="12" t="s">
         <v>76</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="95" spans="1:291" s="5" customFormat="1">
-      <c r="A95" s="15" t="s">
+      <c r="A95" s="12" t="s">
         <v>77</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D95" s="10"/>
       <c r="E95" s="10"/>
@@ -11608,58 +11793,58 @@
       <c r="KE95" s="10"/>
     </row>
     <row r="96" spans="1:291">
-      <c r="A96" s="15" t="s">
+      <c r="A96" s="12" t="s">
         <v>78</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="15" t="s">
+      <c r="A97" s="12" t="s">
         <v>79</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="1" t="s">
+      <c r="A98" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B98" t="s">
-        <v>240</v>
-      </c>
-      <c r="C98" t="s">
-        <v>241</v>
+      <c r="B98" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="1" t="s">
+      <c r="A99" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="6" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="1" t="s">
+      <c r="A100" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B100" t="s">
-        <v>243</v>
-      </c>
-      <c r="C100" t="s">
-        <v>242</v>
+      <c r="B100" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -11668,17 +11853,17 @@
       </c>
       <c r="B101" s="5"/>
       <c r="C101" s="5" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" s="1" t="s">
+      <c r="A102" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="6" t="s">
         <v>94</v>
       </c>
     </row>
@@ -11688,473 +11873,479 @@
       </c>
       <c r="B103" s="5"/>
       <c r="C103" s="5" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B107" s="6" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="C106" s="6" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>253</v>
-      </c>
       <c r="C107" s="6" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="15" t="s">
+      <c r="A108" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="109" spans="1:3">
-      <c r="A109" s="15">
+      <c r="A109" s="12">
         <v>1</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" s="15" t="s">
+      <c r="A110" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="111" spans="1:3">
-      <c r="A111" s="15">
+      <c r="A111" s="12">
         <v>2</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="112" spans="1:3">
-      <c r="A112" s="15" t="s">
+      <c r="A112" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B112" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113" s="15">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="12">
         <v>3</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="C113" s="16" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="A114" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="C113" s="13" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B114" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115" s="15">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="12">
         <v>4</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="C115" s="16" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="C115" s="13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B116" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" s="15">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="12">
         <v>5</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="C117" s="16" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="A118" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="C117" s="13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B118" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="A119" s="15">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="12">
         <v>6</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" s="15" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" s="15">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="12">
         <v>7</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122" s="15" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123" s="15">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="12">
         <v>8</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="A124" s="15" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B124" s="17" t="s">
-        <v>424</v>
-      </c>
-      <c r="C124" s="17" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3">
-      <c r="A125" s="15">
+      <c r="B124" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="C124" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="12">
         <v>9</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3">
-      <c r="A126" s="18" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B126" s="19" t="s">
-        <v>421</v>
-      </c>
-      <c r="C126" s="19" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3">
-      <c r="A127" s="15">
+      <c r="B126" s="16" t="s">
+        <v>409</v>
+      </c>
+      <c r="C126" s="16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="12">
         <v>0</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>14</v>
+        <v>435</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>284</v>
+        <v>436</v>
+      </c>
+      <c r="D128" s="10" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="129" spans="1:4">
-      <c r="A129" s="2" t="s">
+      <c r="A129" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B129" s="3" t="s">
+      <c r="B129" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C129" s="3" t="s">
-        <v>285</v>
+      <c r="C129" s="6" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="130" spans="1:4">
-      <c r="A130" s="15" t="s">
+      <c r="A130" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="131" spans="1:4">
-      <c r="A131" s="15" t="s">
+      <c r="A131" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="132" spans="1:4">
-      <c r="A132" s="15" t="s">
+      <c r="A132" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C132" s="6" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" s="10" customFormat="1">
+      <c r="A133" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C134" s="6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C135" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B137" s="6" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" s="10" customFormat="1">
-      <c r="A133" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B133" s="6" t="s">
+      <c r="C137" s="6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C139" s="6" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B140" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="C133" s="6" t="s">
+      <c r="C140" s="6" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
-      <c r="A134" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B134" s="6" t="s">
+    <row r="141" spans="1:4">
+      <c r="A141" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B141" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="C141" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="C134" s="6" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4">
-      <c r="A135" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B135" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="C135" s="6" t="s">
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="C142" s="6" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
-      <c r="A136" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B136" s="6" t="s">
+    <row r="143" spans="1:4">
+      <c r="A143" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B143" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="C136" s="6" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4">
-      <c r="A137" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B137" s="6" t="s">
+      <c r="C143" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="D143" s="10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="C144" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="C137" s="6" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4">
-      <c r="A138" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B138" s="6" t="s">
-        <v>399</v>
-      </c>
-      <c r="C138" s="6" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4">
-      <c r="A139" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B139" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="C139" s="6" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4">
-      <c r="A140" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B140" s="6" t="s">
+      <c r="D144" s="10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B145" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="C145" s="6" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B146" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="C146" s="17" t="s">
         <v>300</v>
       </c>
-      <c r="C140" s="6" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4">
-      <c r="A141" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B141" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="C141" s="6" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4">
-      <c r="A142" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B142" t="s">
-        <v>304</v>
-      </c>
-      <c r="C142" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4">
-      <c r="A143" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B143" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="C143" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="D143" s="10" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4">
-      <c r="A144" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B144" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="C144" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="D144" s="10" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3">
-      <c r="A145" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B145" s="6" t="s">
-        <v>416</v>
-      </c>
-      <c r="C145" s="6" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3">
-      <c r="A146" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B146" t="s">
-        <v>312</v>
-      </c>
-      <c r="C146" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3">
-      <c r="A147" s="15" t="s">
+      <c r="D146" s="10" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B147" s="6" t="s">
@@ -12164,593 +12355,602 @@
         <v>98</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
-      <c r="A148" s="15" t="s">
+    <row r="148" spans="1:4">
+      <c r="A148" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B148" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="C148" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3">
-      <c r="A149" s="4" t="s">
+      <c r="B148" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="C148" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="D148" s="10" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B149" s="5" t="s">
-        <v>418</v>
-      </c>
-      <c r="C149" s="5" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3">
-      <c r="A150" s="15" t="s">
+      <c r="B149" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="C149" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3">
-      <c r="A151" s="15" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3">
-      <c r="A152" s="15" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3">
-      <c r="A153" s="15" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3">
-      <c r="A154" s="15" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="12" t="s">
         <v>40</v>
       </c>
       <c r="B154" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C154" s="6" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3">
-      <c r="A155" s="15" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="12" t="s">
         <v>41</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" s="10" customFormat="1">
-      <c r="A156" s="15" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" s="10" customFormat="1">
+      <c r="A156" s="12" t="s">
         <v>42</v>
       </c>
       <c r="B156" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C156" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3">
-      <c r="A157" s="15" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="12" t="s">
         <v>43</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
       <c r="A158" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B158" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="D158" s="10" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B159" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C159" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B160" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="C160" s="17" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="C161" s="6" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B162" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C162" s="6" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B163" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="C163" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B164" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C164" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="C158" s="3" t="s">
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B165" s="6" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="159" spans="1:3">
-      <c r="A159" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B159" s="6" t="s">
+      <c r="C165" s="6" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B166" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="C166" s="6" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B167" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C167" s="6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B168" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="C168" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="C159" s="6" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3">
-      <c r="A160" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B160" t="s">
-        <v>330</v>
-      </c>
-      <c r="C160" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3">
-      <c r="A161" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B161" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="C161" s="6" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3">
-      <c r="A162" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B162" s="6" t="s">
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B169" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="C169" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B170" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="C162" s="6" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3">
-      <c r="A163" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B163" t="s">
-        <v>334</v>
-      </c>
-      <c r="C163" t="s">
+      <c r="C170" s="6" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
-      <c r="A164" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B164" s="6" t="s">
+    <row r="171" spans="1:3">
+      <c r="A171" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B171" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="C171" s="17" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B172" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="C172" s="17" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B173" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="C173" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="C164" s="6" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3">
-      <c r="A165" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B165" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="C165" s="6" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3">
-      <c r="A166" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B166" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="C166" s="6" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3">
-      <c r="A167" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B167" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="C167" s="6" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3">
-      <c r="A168" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B168" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="C168" s="6" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3">
-      <c r="A169" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B169" s="6" t="s">
-        <v>392</v>
-      </c>
-      <c r="C169" s="6" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3">
-      <c r="A170" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B170" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="C170" s="6" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3">
-      <c r="A171" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B171" t="s">
-        <v>348</v>
-      </c>
-      <c r="C171" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3">
-      <c r="A172" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B172" t="s">
-        <v>312</v>
-      </c>
-      <c r="C172" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3">
-      <c r="A173" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B173" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="C173" s="6" t="s">
-        <v>349</v>
-      </c>
     </row>
     <row r="174" spans="1:3">
-      <c r="A174" s="15" t="s">
+      <c r="A174" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
     </row>
     <row r="175" spans="1:3">
-      <c r="A175" s="15" t="s">
+      <c r="A175" s="12" t="s">
         <v>61</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
     </row>
     <row r="176" spans="1:3">
-      <c r="A176" s="15" t="s">
+      <c r="A176" s="12" t="s">
         <v>62</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="177" spans="1:3">
-      <c r="A177" s="15" t="s">
+      <c r="A177" s="12" t="s">
         <v>63</v>
       </c>
       <c r="B177" s="6" t="s">
         <v>63</v>
       </c>
       <c r="C177" s="6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B178" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C178" s="6" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B179" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C179" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B180" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="C180" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B181" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="C181" s="6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B182" s="6" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="178" spans="1:3">
-      <c r="A178" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B178" t="s">
-        <v>64</v>
-      </c>
-      <c r="C178" t="s">
+      <c r="C182" s="6" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
-      <c r="A179" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B179" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C179" t="s">
+    <row r="183" spans="1:3">
+      <c r="A183" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B183" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="C183" s="6" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B184" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="C184" s="6" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
-      <c r="A180" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B180" s="6" t="s">
+    <row r="185" spans="1:3">
+      <c r="A185" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B185" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="C185" s="6" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B186" s="5"/>
+      <c r="C186" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="C180" s="6" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3">
-      <c r="A181" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="B181" s="6" t="s">
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B187" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="C187" s="6" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" s="10" customFormat="1">
+      <c r="A188" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B188" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="C188" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="C181" s="6" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3">
-      <c r="A182" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B182" s="6" t="s">
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B189" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="C189" s="17" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B190" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="C190" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="C182" s="6" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3">
-      <c r="A183" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B183" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="C183" s="6" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3">
-      <c r="A184" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B184" s="6" t="s">
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B191" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="C191" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="C184" s="6" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3">
-      <c r="A185" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B185" s="6" t="s">
-        <v>361</v>
-      </c>
-      <c r="C185" s="6" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3">
-      <c r="A186" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B186" t="s">
-        <v>365</v>
-      </c>
-      <c r="C186" s="10" t="s">
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B192" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="C192" s="6" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="187" spans="1:3">
-      <c r="A187" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B187" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="C187" s="6" t="s">
+    <row r="193" spans="1:4">
+      <c r="A193" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B193" s="17" t="s">
+        <v>369</v>
+      </c>
+      <c r="C193" s="17" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="188" spans="1:3" s="10" customFormat="1">
-      <c r="A188" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B188" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="C188" s="6" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3">
-      <c r="A189" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B189" t="s">
-        <v>372</v>
-      </c>
-      <c r="C189" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3">
-      <c r="A190" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B190" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="C190" s="6" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3">
-      <c r="A191" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B191" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="C191" s="6" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3">
-      <c r="A192" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B192" t="s">
-        <v>378</v>
-      </c>
-      <c r="C192" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3">
-      <c r="A193" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B193" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="C193" s="3" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3">
-      <c r="A194" s="15" t="s">
+    <row r="194" spans="1:4">
+      <c r="A194" s="12" t="s">
         <v>80</v>
       </c>
       <c r="B194" s="6" t="s">
         <v>80</v>
       </c>
       <c r="C194" s="6" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
       <c r="A195" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B195" s="13"/>
-      <c r="C195" s="13" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3">
-      <c r="A196" s="15" t="s">
+      <c r="B195" s="6"/>
+      <c r="C195" s="6" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" s="12" t="s">
         <v>82</v>
       </c>
       <c r="B196" s="6" t="s">
         <v>82</v>
       </c>
       <c r="C196" s="6" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3">
-      <c r="A197" s="12" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B197" s="13"/>
-      <c r="C197" s="13" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3">
-      <c r="A198" s="8" t="s">
+      <c r="B197" s="17" t="s">
+        <v>443</v>
+      </c>
+      <c r="C197" s="17" t="s">
+        <v>442</v>
+      </c>
+      <c r="D197" s="10" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B198" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C198" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3">
-      <c r="A199" s="8" t="s">
+      <c r="C198" s="6" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B199" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C199" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3">
+      <c r="C199" s="6" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
       <c r="A200" s="8"/>
     </row>
-    <row r="201" spans="1:3">
+    <row r="201" spans="1:4">
       <c r="A201" s="8"/>
     </row>
-    <row r="202" spans="1:3">
+    <row r="202" spans="1:4">
       <c r="A202" s="8"/>
     </row>
-    <row r="203" spans="1:3">
+    <row r="203" spans="1:4">
       <c r="A203" s="8"/>
     </row>
-    <row r="204" spans="1:3">
+    <row r="204" spans="1:4">
       <c r="A204" s="8"/>
     </row>
-    <row r="205" spans="1:3">
+    <row r="205" spans="1:4">
       <c r="A205" s="8"/>
     </row>
-    <row r="206" spans="1:3">
+    <row r="206" spans="1:4">
       <c r="A206" s="8"/>
     </row>
   </sheetData>

</xml_diff>